<commit_message>
"added shuffle to unknown, fixed vocabulary bugs"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55A6FD48-153C-4C70-BDFA-1C3BF9E79D00}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DA701C-1BDD-FB4C-A066-2EAAEB4723A3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$C$122</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="237">
   <si>
     <t>Griechisch</t>
   </si>
@@ -74,9 +74,6 @@
     <t>das Handy</t>
   </si>
   <si>
-    <t>guten Tag / Abend</t>
-  </si>
-  <si>
     <t>Spruch</t>
   </si>
   <si>
@@ -515,9 +512,6 @@
     <t>sie (m)</t>
   </si>
   <si>
-    <t>sie (f)</t>
-  </si>
-  <si>
     <t>sie (n)</t>
   </si>
   <si>
@@ -602,9 +596,6 @@
     <t>Guten Tag (formell)</t>
   </si>
   <si>
-    <t>guten Morgen / Tag</t>
-  </si>
-  <si>
     <t>Καλημέρα</t>
   </si>
   <si>
@@ -617,9 +608,6 @@
     <t>Sehr gut. Und dir?</t>
   </si>
   <si>
-    <t>Mir / uns geht es gut</t>
-  </si>
-  <si>
     <t>Es geht</t>
   </si>
   <si>
@@ -629,18 +617,12 @@
     <t>πολύ καλά. Εσύ;</t>
   </si>
   <si>
-    <t>Είμαι / Είμαστε καλά</t>
-  </si>
-  <si>
     <t>Έτσι κι έτσι</t>
   </si>
   <si>
     <t>Χάλια</t>
   </si>
   <si>
-    <t>γεια σου / σας, Αντίο</t>
-  </si>
-  <si>
     <t>Καλό μεσημέρι</t>
   </si>
   <si>
@@ -650,9 +632,6 @@
     <t>Καλό βράδυ</t>
   </si>
   <si>
-    <t>Tschüss / Auf Wiedersehen</t>
-  </si>
-  <si>
     <t>Schönen Mittag</t>
   </si>
   <si>
@@ -665,9 +644,6 @@
     <t>Zahlen</t>
   </si>
   <si>
-    <t>Lehrbuch 2</t>
-  </si>
-  <si>
     <t>μηδέν</t>
   </si>
   <si>
@@ -729,6 +705,27 @@
   </si>
   <si>
     <t>είκοσι</t>
+  </si>
+  <si>
+    <t>sie (pl, f)</t>
+  </si>
+  <si>
+    <t>guten Morgen | Tag</t>
+  </si>
+  <si>
+    <t>guten Tag | Abend</t>
+  </si>
+  <si>
+    <t>Mir | uns geht es gut</t>
+  </si>
+  <si>
+    <t>Tschüss | Auf Wiedersehen</t>
+  </si>
+  <si>
+    <t>Είμαι | Είμαστε καλά</t>
+  </si>
+  <si>
+    <t>γεια σου | σας, Αντίο</t>
   </si>
 </sst>
 </file>
@@ -1106,16 +1103,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="18.265625" customWidth="1"/>
+    <col min="1" max="4" width="18.203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,51 +1126,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>150</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1185,9 +1182,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1199,12 +1196,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1213,12 +1210,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1227,12 +1224,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1241,12 +1238,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1255,12 +1252,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1269,12 +1266,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1283,12 +1280,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1297,12 +1294,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1311,12 +1308,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1325,12 +1322,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1339,12 +1336,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1353,12 +1350,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1367,9 +1364,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -1381,9 +1378,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -1395,12 +1392,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1409,12 +1406,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1423,12 +1420,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1437,1115 +1434,1115 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
         <v>140</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" t="s">
-        <v>69</v>
-      </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
         <v>148</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>76</v>
       </c>
-      <c r="C36" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>92</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>168</v>
+      </c>
+      <c r="B58" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" t="s">
+        <v>223</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>83</v>
+      </c>
+      <c r="B61" t="s">
+        <v>224</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
         <v>21</v>
       </c>
-      <c r="C40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>161</v>
-      </c>
-      <c r="B44" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" t="s">
-        <v>157</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>163</v>
-      </c>
-      <c r="B46" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47" t="s">
-        <v>159</v>
-      </c>
-      <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>93</v>
-      </c>
-      <c r="B48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" t="s">
+        <v>184</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
         <v>104</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B64" t="s">
         <v>35</v>
       </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>166</v>
-      </c>
-      <c r="B53" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>167</v>
-      </c>
-      <c r="B55" t="s">
-        <v>174</v>
-      </c>
-      <c r="C55" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" t="s">
+        <v>187</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" t="s">
+        <v>225</v>
+      </c>
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>193</v>
+      </c>
+      <c r="B71" t="s">
+        <v>190</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
         <v>175</v>
       </c>
-      <c r="C56" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>169</v>
-      </c>
-      <c r="B57" t="s">
-        <v>176</v>
-      </c>
-      <c r="C57" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>170</v>
-      </c>
-      <c r="B58" t="s">
-        <v>172</v>
-      </c>
-      <c r="C58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>171</v>
-      </c>
-      <c r="B59" t="s">
-        <v>173</v>
-      </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>188</v>
-      </c>
-      <c r="B60" t="s">
-        <v>187</v>
-      </c>
-      <c r="C60" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="B73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" t="s">
         <v>11</v>
       </c>
-      <c r="C61" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>184</v>
-      </c>
-      <c r="B62" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>185</v>
-      </c>
-      <c r="B63" t="s">
-        <v>186</v>
-      </c>
-      <c r="C63" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>105</v>
-      </c>
-      <c r="B64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>133</v>
-      </c>
-      <c r="B65" t="s">
-        <v>189</v>
-      </c>
-      <c r="C65" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>124</v>
-      </c>
-      <c r="B66" t="s">
-        <v>190</v>
-      </c>
-      <c r="C66" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>179</v>
+      </c>
+      <c r="B75" t="s">
+        <v>178</v>
+      </c>
+      <c r="C75" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>181</v>
+      </c>
+      <c r="B76" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>228</v>
+      </c>
+      <c r="B78" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79" t="s">
+        <v>197</v>
+      </c>
+      <c r="C79" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
         <v>195</v>
       </c>
-      <c r="B67" t="s">
-        <v>191</v>
-      </c>
-      <c r="C67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+      <c r="B80" t="s">
+        <v>198</v>
+      </c>
+      <c r="C80" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
         <v>196</v>
       </c>
-      <c r="B69" t="s">
-        <v>192</v>
-      </c>
-      <c r="C69" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>197</v>
-      </c>
-      <c r="B70" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>198</v>
-      </c>
-      <c r="B71" t="s">
-        <v>194</v>
-      </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" t="s">
-        <v>41</v>
-      </c>
-      <c r="C72" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>177</v>
-      </c>
-      <c r="B73" t="s">
-        <v>50</v>
-      </c>
-      <c r="C73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" t="s">
-        <v>52</v>
-      </c>
-      <c r="C74" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>181</v>
-      </c>
-      <c r="B75" t="s">
-        <v>180</v>
-      </c>
-      <c r="C75" t="s">
-        <v>12</v>
-      </c>
-      <c r="D75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>183</v>
-      </c>
-      <c r="B76" t="s">
-        <v>182</v>
-      </c>
-      <c r="C76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>132</v>
-      </c>
-      <c r="B77" t="s">
-        <v>63</v>
-      </c>
-      <c r="C77" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+      <c r="B81" t="s">
         <v>199</v>
       </c>
-      <c r="B78" t="s">
-        <v>203</v>
-      </c>
-      <c r="C78" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>200</v>
-      </c>
-      <c r="B79" t="s">
-        <v>204</v>
-      </c>
-      <c r="C79" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+      <c r="C81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
         <v>201</v>
-      </c>
-      <c r="B80" t="s">
-        <v>205</v>
-      </c>
-      <c r="C80" t="s">
-        <v>12</v>
-      </c>
-      <c r="D80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>202</v>
-      </c>
-      <c r="B81" t="s">
-        <v>206</v>
-      </c>
-      <c r="C81" t="s">
-        <v>12</v>
-      </c>
-      <c r="D81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>209</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D82" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D83" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B84">
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D85" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B86">
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D86" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B87">
         <v>5</v>
       </c>
       <c r="C87" t="s">
+        <v>200</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
         <v>207</v>
-      </c>
-      <c r="D87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>215</v>
       </c>
       <c r="B88">
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D88" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B89">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D89" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B90">
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B91">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D91" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B92">
         <v>10</v>
       </c>
       <c r="C92" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D92" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B93">
         <v>11</v>
       </c>
       <c r="C93" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B94">
         <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D94" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B95">
         <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D95" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B96">
         <v>14</v>
       </c>
       <c r="C96" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B97">
         <v>15</v>
       </c>
       <c r="C97" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D97" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B98">
         <v>16</v>
       </c>
       <c r="C98" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D98" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B99">
         <v>17</v>
       </c>
       <c r="C99" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D99" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B100">
         <v>18</v>
       </c>
       <c r="C100" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D100" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B101">
         <v>19</v>
       </c>
       <c r="C101" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D101" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B102">
         <v>20</v>
       </c>
       <c r="C102" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D102" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
@@ -2557,12 +2554,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B104" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -2571,12 +2568,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B105" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C105" t="s">
         <v>6</v>
@@ -2585,12 +2582,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C106" t="s">
         <v>6</v>
@@ -2599,12 +2596,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B107" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C107" t="s">
         <v>6</v>
@@ -2613,12 +2610,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B108" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
@@ -2627,12 +2624,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B109" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
@@ -2641,12 +2638,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C110" t="s">
         <v>6</v>
@@ -2655,12 +2652,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
@@ -2669,12 +2666,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
@@ -2683,12 +2680,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
@@ -2697,12 +2694,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
@@ -2711,12 +2708,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
@@ -2725,12 +2722,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C116" t="s">
         <v>6</v>
@@ -2739,12 +2736,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B117" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
@@ -2753,12 +2750,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B118" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -2767,12 +2764,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B119" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C119" t="s">
         <v>6</v>
@@ -2781,12 +2778,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B120" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C120" t="s">
         <v>6</v>
@@ -2795,12 +2792,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B121" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C121" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
"added chapter 2 voci"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DA701C-1BDD-FB4C-A066-2EAAEB4723A3}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F74CFB2D-FDA5-49D4-9B01-5EDACDEA8B0D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="444">
   <si>
     <t>Griechisch</t>
   </si>
@@ -404,9 +404,6 @@
     <t>χάνω</t>
   </si>
   <si>
-    <t>ακόμη / ακόμα</t>
-  </si>
-  <si>
     <t>το παιδί</t>
   </si>
   <si>
@@ -587,9 +584,6 @@
     <t>Χαίρω πολύ</t>
   </si>
   <si>
-    <t>γεια σου / σας</t>
-  </si>
-  <si>
     <t>Χαίρετε</t>
   </si>
   <si>
@@ -665,9 +659,6 @@
     <t>έξι</t>
   </si>
   <si>
-    <t>εφτά / επτά</t>
-  </si>
-  <si>
     <t>οκτώ οχτώ</t>
   </si>
   <si>
@@ -677,9 +668,6 @@
     <t>δέκα</t>
   </si>
   <si>
-    <t>έντεκα ένδεκα</t>
-  </si>
-  <si>
     <t>δώδεκα</t>
   </si>
   <si>
@@ -692,18 +680,6 @@
     <t>δεκαπέντε</t>
   </si>
   <si>
-    <t>δεκαέξι δεκάξι</t>
-  </si>
-  <si>
-    <t>δεκαεφτά δεκαεπτά</t>
-  </si>
-  <si>
-    <t>δεκαοκτώ δεκαοχτώ</t>
-  </si>
-  <si>
-    <t>δεκαεννιά δεκαεννέα</t>
-  </si>
-  <si>
     <t>είκοσι</t>
   </si>
   <si>
@@ -726,6 +702,675 @@
   </si>
   <si>
     <t>γεια σου | σας, Αντίο</t>
+  </si>
+  <si>
+    <t>ακόμη | ακόμα</t>
+  </si>
+  <si>
+    <t>γεια σου | σας</t>
+  </si>
+  <si>
+    <t>εφτά | επτά</t>
+  </si>
+  <si>
+    <t>έντεκα | ένδεκα</t>
+  </si>
+  <si>
+    <t>δεκαέξι | δεκάξι</t>
+  </si>
+  <si>
+    <t>δεκαεφτά | δεκαεπτά</t>
+  </si>
+  <si>
+    <t>δεκαοκτώ | δεκαοχτώ</t>
+  </si>
+  <si>
+    <t>δεκαεννιά | δεκαεννέα</t>
+  </si>
+  <si>
+    <t>ο πινακας ανακοινώσεων</t>
+  </si>
+  <si>
+    <t>das schwarze Brett</t>
+  </si>
+  <si>
+    <t>Lehrbuch 2</t>
+  </si>
+  <si>
+    <t>η κοπέλα</t>
+  </si>
+  <si>
+    <t>die junge Frau</t>
+  </si>
+  <si>
+    <t>η κατεπίνη</t>
+  </si>
+  <si>
+    <t>Katerini (Stadt)</t>
+  </si>
+  <si>
+    <t>η ιατρική</t>
+  </si>
+  <si>
+    <t>die Medizin</t>
+  </si>
+  <si>
+    <t>το διαμέρισμα</t>
+  </si>
+  <si>
+    <t>das Appartement</t>
+  </si>
+  <si>
+    <t>in, auf, an, bei, nach, zu</t>
+  </si>
+  <si>
+    <t>τηλ.</t>
+  </si>
+  <si>
+    <t>Tel.</t>
+  </si>
+  <si>
+    <t>το τηλέφωνο</t>
+  </si>
+  <si>
+    <t>das Telefon</t>
+  </si>
+  <si>
+    <t>έχω</t>
+  </si>
+  <si>
+    <t>haben</t>
+  </si>
+  <si>
+    <t>τα έπιπλα</t>
+  </si>
+  <si>
+    <t>das Möbel</t>
+  </si>
+  <si>
+    <t>ποιος</t>
+  </si>
+  <si>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>πουλάω</t>
+  </si>
+  <si>
+    <t>verkaufen</t>
+  </si>
+  <si>
+    <t>ή</t>
+  </si>
+  <si>
+    <t>oder</t>
+  </si>
+  <si>
+    <t>χαρίζω</t>
+  </si>
+  <si>
+    <t>(ver)schenken</t>
+  </si>
+  <si>
+    <t>η καρέκλα</t>
+  </si>
+  <si>
+    <t>der Stuhl</t>
+  </si>
+  <si>
+    <t>το τραπέζι</t>
+  </si>
+  <si>
+    <t>der Tisch</t>
+  </si>
+  <si>
+    <t>το κρεβάτι</t>
+  </si>
+  <si>
+    <t>das Bett</t>
+  </si>
+  <si>
+    <t>die Handynummer</t>
+  </si>
+  <si>
+    <t>μου</t>
+  </si>
+  <si>
+    <t>mein</t>
+  </si>
+  <si>
+    <t>μετακομίζω</t>
+  </si>
+  <si>
+    <t>umziehen</t>
+  </si>
+  <si>
+    <t>ο δισκος</t>
+  </si>
+  <si>
+    <t>die Schallplatte</t>
+  </si>
+  <si>
+    <t>το σιντί</t>
+  </si>
+  <si>
+    <t>die CD</t>
+  </si>
+  <si>
+    <t>άλλα</t>
+  </si>
+  <si>
+    <t>andere</t>
+  </si>
+  <si>
+    <t>το πράγμα</t>
+  </si>
+  <si>
+    <t>die Sache, das Ding</t>
+  </si>
+  <si>
+    <t>ο δικηγόρος</t>
+  </si>
+  <si>
+    <t>der Rechtsanwalt</t>
+  </si>
+  <si>
+    <t>...χρονών</t>
+  </si>
+  <si>
+    <t>… Jahre alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> προτιμάω</t>
+  </si>
+  <si>
+    <t>bevorzugen</t>
+  </si>
+  <si>
+    <t>η φοιτήτρια</t>
+  </si>
+  <si>
+    <t>die Studentin</t>
+  </si>
+  <si>
+    <t>γιατί</t>
+  </si>
+  <si>
+    <t>warum, weil</t>
+  </si>
+  <si>
+    <t>γελάω</t>
+  </si>
+  <si>
+    <t>lachen</t>
+  </si>
+  <si>
+    <t>κάνω πλάκα</t>
+  </si>
+  <si>
+    <t>Spass machen</t>
+  </si>
+  <si>
+    <t>der Angestellte</t>
+  </si>
+  <si>
+    <t>η τράπεζα</t>
+  </si>
+  <si>
+    <t>die Bank</t>
+  </si>
+  <si>
+    <t>η γυναίκα</t>
+  </si>
+  <si>
+    <t>die Frau, Ehefrau</t>
+  </si>
+  <si>
+    <t>ζητάω</t>
+  </si>
+  <si>
+    <t>suchen nach, verlangen</t>
+  </si>
+  <si>
+    <t>η μπέιμπι σίτερ</t>
+  </si>
+  <si>
+    <t>die Babysitterin</t>
+  </si>
+  <si>
+    <t>για</t>
+  </si>
+  <si>
+    <t>für</t>
+  </si>
+  <si>
+    <t>η κόρη</t>
+  </si>
+  <si>
+    <t>die Tochter</t>
+  </si>
+  <si>
+    <t>μας</t>
+  </si>
+  <si>
+    <t>unser</t>
+  </si>
+  <si>
+    <t>η Ισπανίδα</t>
+  </si>
+  <si>
+    <t>die Spanierin</t>
+  </si>
+  <si>
+    <t>η βοήθεια</t>
+  </si>
+  <si>
+    <t>die Hilfe</t>
+  </si>
+  <si>
+    <t>τα λεφτά</t>
+  </si>
+  <si>
+    <t>das Geld</t>
+  </si>
+  <si>
+    <t>η δουλειά</t>
+  </si>
+  <si>
+    <t>die Arbeit</t>
+  </si>
+  <si>
+    <t>η Μαδρίτη</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>μιλάω</t>
+  </si>
+  <si>
+    <t>sprechen, reden</t>
+  </si>
+  <si>
+    <t>τα αγγλικά</t>
+  </si>
+  <si>
+    <t>Englisch</t>
+  </si>
+  <si>
+    <t>φυσικά</t>
+  </si>
+  <si>
+    <t>natürlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjektiv </t>
+  </si>
+  <si>
+    <t>τα Ισπανικά</t>
+  </si>
+  <si>
+    <t>Spanisch</t>
+  </si>
+  <si>
+    <t>αγαπάω</t>
+  </si>
+  <si>
+    <t>lieben, mögen</t>
+  </si>
+  <si>
+    <t>η γλώσσα</t>
+  </si>
+  <si>
+    <t>die Sprache</t>
+  </si>
+  <si>
+    <t>οι ξένες γλώσσες</t>
+  </si>
+  <si>
+    <t>die Fremdsprache</t>
+  </si>
+  <si>
+    <t>αν</t>
+  </si>
+  <si>
+    <t>wenn, falls, ob</t>
+  </si>
+  <si>
+    <t>η δασκάλα</t>
+  </si>
+  <si>
+    <t>die Lehrerin</t>
+  </si>
+  <si>
+    <t>κάνω παζάρια</t>
+  </si>
+  <si>
+    <t>feilschen, handeln</t>
+  </si>
+  <si>
+    <t>η αγγελία</t>
+  </si>
+  <si>
+    <t>die Anzeige</t>
+  </si>
+  <si>
+    <t>παίρνω τηλέφωνο</t>
+  </si>
+  <si>
+    <t>anrufen</t>
+  </si>
+  <si>
+    <t>ο κύριος</t>
+  </si>
+  <si>
+    <t>Herr</t>
+  </si>
+  <si>
+    <t>παρακαλώ</t>
+  </si>
+  <si>
+    <t>bitte</t>
+  </si>
+  <si>
+    <t>τηλεφωνώ</t>
+  </si>
+  <si>
+    <t>telefonieren</t>
+  </si>
+  <si>
+    <t>επειδή</t>
+  </si>
+  <si>
+    <t>weil, da</t>
+  </si>
+  <si>
+    <t>μάλιστα</t>
+  </si>
+  <si>
+    <t>richtig, jawohl</t>
+  </si>
+  <si>
+    <t>ο ξένος</t>
+  </si>
+  <si>
+    <t>der Ausländer</t>
+  </si>
+  <si>
+    <t>μπράβο</t>
+  </si>
+  <si>
+    <t>bravo</t>
+  </si>
+  <si>
+    <t>δουλεύω</t>
+  </si>
+  <si>
+    <t>arbeiten</t>
+  </si>
+  <si>
+    <t>η Ελλάδα</t>
+  </si>
+  <si>
+    <t>Griechenland</t>
+  </si>
+  <si>
+    <t>ζω</t>
+  </si>
+  <si>
+    <t>leben</t>
+  </si>
+  <si>
+    <t>χωρίς</t>
+  </si>
+  <si>
+    <t>ohne</t>
+  </si>
+  <si>
+    <t>πού</t>
+  </si>
+  <si>
+    <t>wo</t>
+  </si>
+  <si>
+    <t>τρώω</t>
+  </si>
+  <si>
+    <t>essen</t>
+  </si>
+  <si>
+    <t>το πάτωμα</t>
+  </si>
+  <si>
+    <t>der Fussboden</t>
+  </si>
+  <si>
+    <t>μένω</t>
+  </si>
+  <si>
+    <t>wohnen</t>
+  </si>
+  <si>
+    <t>η φίλη</t>
+  </si>
+  <si>
+    <t>die Freundin</t>
+  </si>
+  <si>
+    <t>αύπιο</t>
+  </si>
+  <si>
+    <t>morgen</t>
+  </si>
+  <si>
+    <t>από αύπιο</t>
+  </si>
+  <si>
+    <t>ab morgen</t>
+  </si>
+  <si>
+    <t>συγνώμη</t>
+  </si>
+  <si>
+    <t>Verzeihung</t>
+  </si>
+  <si>
+    <t>η Ελληνίδα</t>
+  </si>
+  <si>
+    <t>die Griechin</t>
+  </si>
+  <si>
+    <t>η Γερμανίδα</t>
+  </si>
+  <si>
+    <t>die Deutsche</t>
+  </si>
+  <si>
+    <t>τη λένε</t>
+  </si>
+  <si>
+    <t>sie heisst</t>
+  </si>
+  <si>
+    <t>η καθηγήτρια</t>
+  </si>
+  <si>
+    <t>die Gymnasiallehrerin</t>
+  </si>
+  <si>
+    <t>τα γαλλικά</t>
+  </si>
+  <si>
+    <t>Französisch</t>
+  </si>
+  <si>
+    <t>τα ιταλικά</t>
+  </si>
+  <si>
+    <t>Italienisch</t>
+  </si>
+  <si>
+    <t>η λάμπα</t>
+  </si>
+  <si>
+    <t>die Lampe</t>
+  </si>
+  <si>
+    <t>η κατσαρόλα</t>
+  </si>
+  <si>
+    <t>der Kochtopf</t>
+  </si>
+  <si>
+    <t>η σκούπα</t>
+  </si>
+  <si>
+    <t>θέλω</t>
+  </si>
+  <si>
+    <t>wollen, mögen</t>
+  </si>
+  <si>
+    <t>εντάξει</t>
+  </si>
+  <si>
+    <t>in Ordnung</t>
+  </si>
+  <si>
+    <t>φεύγω</t>
+  </si>
+  <si>
+    <t>verlassen, weggehen</t>
+  </si>
+  <si>
+    <t>η Δευτέρα</t>
+  </si>
+  <si>
+    <t>Montag</t>
+  </si>
+  <si>
+    <t>τι να κάνω</t>
+  </si>
+  <si>
+    <t>was soll ich machen</t>
+  </si>
+  <si>
+    <t>το πιάτο</t>
+  </si>
+  <si>
+    <t>der Teller</t>
+  </si>
+  <si>
+    <t>το κουτάλι</t>
+  </si>
+  <si>
+    <t>der Löffel</t>
+  </si>
+  <si>
+    <t>το πιρούνι</t>
+  </si>
+  <si>
+    <t>die Gabel</t>
+  </si>
+  <si>
+    <t>το μαχαίρι</t>
+  </si>
+  <si>
+    <t>das Messer</t>
+  </si>
+  <si>
+    <t>ο φούρνος</t>
+  </si>
+  <si>
+    <t>der Backofen</t>
+  </si>
+  <si>
+    <t>ούτε ... oύτε</t>
+  </si>
+  <si>
+    <t>weder … noch</t>
+  </si>
+  <si>
+    <t>πενήντα</t>
+  </si>
+  <si>
+    <t>fünfzig</t>
+  </si>
+  <si>
+    <t>το ευρώ</t>
+  </si>
+  <si>
+    <t>der Euro</t>
+  </si>
+  <si>
+    <t>αγοράζω</t>
+  </si>
+  <si>
+    <t>kaufen</t>
+  </si>
+  <si>
+    <t>το νοικοκυριό</t>
+  </si>
+  <si>
+    <t>der Haushalt</t>
+  </si>
+  <si>
+    <t>παίρνω</t>
+  </si>
+  <si>
+    <t>nehmen</t>
+  </si>
+  <si>
+    <t>η πόρτα</t>
+  </si>
+  <si>
+    <t>die Tür</t>
+  </si>
+  <si>
+    <t>το παράθυρο</t>
+  </si>
+  <si>
+    <t>das Fenster</t>
+  </si>
+  <si>
+    <t>ο ανεμιστήρας</t>
+  </si>
+  <si>
+    <t>der Ventilator</t>
+  </si>
+  <si>
+    <t>πολύ</t>
+  </si>
+  <si>
+    <t>sehr</t>
+  </si>
+  <si>
+    <t>το απόγευμα</t>
+  </si>
+  <si>
+    <t>am Nachmittag</t>
+  </si>
+  <si>
+    <t>στον | στι</t>
+  </si>
+  <si>
+    <t>ο | η συγκάτοικος</t>
+  </si>
+  <si>
+    <t>der | die Mitbewohner</t>
+  </si>
+  <si>
+    <t>ο | η υπάλληλος</t>
+  </si>
+  <si>
+    <t>ο | η γραμματέας</t>
+  </si>
+  <si>
+    <t>der | die Sekretär</t>
+  </si>
+  <si>
+    <t>der Besen | der Staubsauger</t>
   </si>
 </sst>
 </file>
@@ -765,8 +1410,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1101,22 +1748,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A108" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="18.203125" customWidth="1"/>
+    <col min="1" max="2" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1126,12 +1774,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B2" t="s">
-        <v>152</v>
+      <c r="B2" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -1140,11 +1788,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="s">
@@ -1154,11 +1802,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
@@ -1168,11 +1816,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
@@ -1182,11 +1830,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
@@ -1196,11 +1844,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
@@ -1210,11 +1858,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
@@ -1224,11 +1872,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
@@ -1238,11 +1886,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C10" t="s">
@@ -1252,11 +1900,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C11" t="s">
@@ -1266,11 +1914,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
@@ -1280,11 +1928,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C13" t="s">
@@ -1294,11 +1942,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" t="s">
@@ -1308,11 +1956,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C15" t="s">
@@ -1322,11 +1970,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C16" t="s">
@@ -1336,11 +1984,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C17" t="s">
@@ -1350,11 +1998,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C18" t="s">
@@ -1364,25 +2012,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C20" t="s">
@@ -1392,11 +2040,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>142</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C21" t="s">
@@ -1406,25 +2054,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C23" t="s">
@@ -1434,11 +2082,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C24" t="s">
@@ -1448,12 +2096,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B25" t="s">
-        <v>177</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
@@ -1462,11 +2110,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C26" t="s">
@@ -1476,11 +2124,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C27" t="s">
@@ -1490,11 +2138,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
@@ -1504,11 +2152,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C29" t="s">
@@ -1518,11 +2166,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C30" t="s">
@@ -1532,11 +2180,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>133</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C31" t="s">
@@ -1546,11 +2194,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>137</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C32" t="s">
@@ -1560,11 +2208,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C33" t="s">
@@ -1574,11 +2222,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C34" t="s">
@@ -1588,11 +2236,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>143</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C35" t="s">
@@ -1602,11 +2250,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C36" t="s">
@@ -1616,11 +2264,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C37" t="s">
@@ -1630,11 +2278,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
@@ -1644,11 +2292,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
@@ -1658,11 +2306,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C40" t="s">
@@ -1672,11 +2320,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C41" t="s">
@@ -1686,11 +2334,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>129</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C42" t="s">
@@ -1700,11 +2348,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>158</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C43" t="s">
@@ -1714,12 +2362,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>159</v>
-      </c>
-      <c r="B44" t="s">
-        <v>155</v>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
@@ -1728,12 +2376,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" t="s">
-        <v>156</v>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
@@ -1742,12 +2390,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" t="s">
-        <v>222</v>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
@@ -1756,12 +2404,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" t="s">
-        <v>157</v>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -1770,11 +2418,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C48" t="s">
@@ -1784,11 +2432,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C49" t="s">
@@ -1798,11 +2446,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C50" t="s">
@@ -1812,11 +2460,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C51" t="s">
@@ -1826,12 +2474,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>163</v>
-      </c>
-      <c r="B52" t="s">
-        <v>153</v>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="C52" t="s">
         <v>13</v>
@@ -1840,12 +2488,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
-        <v>164</v>
-      </c>
-      <c r="B53" t="s">
-        <v>154</v>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="C53" t="s">
         <v>13</v>
@@ -1854,11 +2502,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
-        <v>127</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C54" t="s">
@@ -1868,12 +2516,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
-        <v>165</v>
-      </c>
-      <c r="B55" t="s">
-        <v>172</v>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
@@ -1882,12 +2530,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>166</v>
-      </c>
-      <c r="B56" t="s">
-        <v>173</v>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="C56" t="s">
         <v>13</v>
@@ -1896,12 +2544,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
-        <v>167</v>
-      </c>
-      <c r="B57" t="s">
-        <v>174</v>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C57" t="s">
         <v>13</v>
@@ -1910,12 +2558,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
-        <v>168</v>
-      </c>
-      <c r="B58" t="s">
-        <v>170</v>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="C58" t="s">
         <v>13</v>
@@ -1924,12 +2572,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
-        <v>169</v>
-      </c>
-      <c r="B59" t="s">
-        <v>171</v>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C59" t="s">
         <v>13</v>
@@ -1938,12 +2586,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" t="s">
-        <v>185</v>
-      </c>
-      <c r="B60" t="s">
-        <v>223</v>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
@@ -1952,12 +2600,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B61" t="s">
-        <v>224</v>
+      <c r="B61" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="C61" t="s">
         <v>11</v>
@@ -1966,11 +2614,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
-        <v>182</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C62" t="s">
@@ -1980,12 +2628,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" t="s">
-        <v>184</v>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -1994,11 +2642,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C64" t="s">
@@ -2008,12 +2656,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
-        <v>132</v>
-      </c>
-      <c r="B65" t="s">
-        <v>186</v>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -2022,12 +2670,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" t="s">
-        <v>187</v>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -2036,12 +2684,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
-        <v>191</v>
-      </c>
-      <c r="B67" t="s">
-        <v>188</v>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -2050,11 +2698,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" t="s">
-        <v>124</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C68" t="s">
@@ -2064,12 +2712,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" t="s">
-        <v>227</v>
-      </c>
-      <c r="B69" t="s">
-        <v>225</v>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
@@ -2078,12 +2726,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" t="s">
-        <v>192</v>
-      </c>
-      <c r="B70" t="s">
-        <v>189</v>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="C70" t="s">
         <v>11</v>
@@ -2092,12 +2740,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" t="s">
-        <v>193</v>
-      </c>
-      <c r="B71" t="s">
-        <v>190</v>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="C71" t="s">
         <v>11</v>
@@ -2106,11 +2754,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C72" t="s">
@@ -2120,11 +2768,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" t="s">
-        <v>175</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C73" t="s">
@@ -2134,11 +2782,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C74" t="s">
@@ -2148,12 +2796,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" t="s">
-        <v>179</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
         <v>178</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -2162,12 +2810,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" t="s">
-        <v>181</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>180</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -2176,11 +2824,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A77" t="s">
-        <v>131</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C77" t="s">
@@ -2190,12 +2838,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A78" t="s">
-        <v>228</v>
-      </c>
-      <c r="B78" t="s">
-        <v>226</v>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="C78" t="s">
         <v>11</v>
@@ -2204,12 +2852,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A79" t="s">
-        <v>194</v>
-      </c>
-      <c r="B79" t="s">
-        <v>197</v>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="C79" t="s">
         <v>11</v>
@@ -2218,12 +2866,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A80" t="s">
-        <v>195</v>
-      </c>
-      <c r="B80" t="s">
-        <v>198</v>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
@@ -2232,12 +2880,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" t="s">
-        <v>196</v>
-      </c>
-      <c r="B81" t="s">
-        <v>199</v>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="C81" t="s">
         <v>11</v>
@@ -2246,305 +2894,305 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>198</v>
+      </c>
+      <c r="D82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82" t="s">
-        <v>200</v>
-      </c>
-      <c r="D82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83" t="s">
+      <c r="B84" s="2">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>198</v>
+      </c>
+      <c r="D84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-      <c r="C83" t="s">
-        <v>200</v>
-      </c>
-      <c r="D83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" t="s">
+      <c r="B85" s="2">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>198</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B84">
-        <v>2</v>
-      </c>
-      <c r="C84" t="s">
-        <v>200</v>
-      </c>
-      <c r="D84" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85" t="s">
+      <c r="B86" s="2">
+        <v>4</v>
+      </c>
+      <c r="C86" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B85">
-        <v>3</v>
-      </c>
-      <c r="C85" t="s">
-        <v>200</v>
-      </c>
-      <c r="D85" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A86" t="s">
+      <c r="B87" s="2">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>198</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B86">
-        <v>4</v>
-      </c>
-      <c r="C86" t="s">
-        <v>200</v>
-      </c>
-      <c r="D86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87" t="s">
+      <c r="B88" s="2">
+        <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>198</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B89" s="2">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B87">
-        <v>5</v>
-      </c>
-      <c r="C87" t="s">
-        <v>200</v>
-      </c>
-      <c r="D87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" t="s">
+      <c r="B90" s="2">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>198</v>
+      </c>
+      <c r="D90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B88">
-        <v>6</v>
-      </c>
-      <c r="C88" t="s">
-        <v>200</v>
-      </c>
-      <c r="D88" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89" t="s">
+      <c r="B91" s="2">
+        <v>9</v>
+      </c>
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B89">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s">
-        <v>200</v>
-      </c>
-      <c r="D89" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" t="s">
+      <c r="B92" s="2">
+        <v>10</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+      <c r="D92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B93" s="2">
+        <v>11</v>
+      </c>
+      <c r="C93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B90">
-        <v>8</v>
-      </c>
-      <c r="C90" t="s">
-        <v>200</v>
-      </c>
-      <c r="D90" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91" t="s">
+      <c r="B94" s="2">
+        <v>12</v>
+      </c>
+      <c r="C94" t="s">
+        <v>198</v>
+      </c>
+      <c r="D94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B91">
-        <v>9</v>
-      </c>
-      <c r="C91" t="s">
-        <v>200</v>
-      </c>
-      <c r="D91" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92" t="s">
+      <c r="B95" s="2">
+        <v>13</v>
+      </c>
+      <c r="C95" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B92">
-        <v>10</v>
-      </c>
-      <c r="C92" t="s">
-        <v>200</v>
-      </c>
-      <c r="D92" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93" t="s">
+      <c r="B96" s="2">
+        <v>14</v>
+      </c>
+      <c r="C96" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B93">
-        <v>11</v>
-      </c>
-      <c r="C93" t="s">
-        <v>200</v>
-      </c>
-      <c r="D93" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A94" t="s">
+      <c r="B97" s="2">
+        <v>15</v>
+      </c>
+      <c r="C97" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B98" s="2">
+        <v>16</v>
+      </c>
+      <c r="C98" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B99" s="2">
+        <v>17</v>
+      </c>
+      <c r="C99" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B100" s="2">
+        <v>18</v>
+      </c>
+      <c r="C100" t="s">
+        <v>198</v>
+      </c>
+      <c r="D100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B101" s="2">
+        <v>19</v>
+      </c>
+      <c r="C101" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B94">
-        <v>12</v>
-      </c>
-      <c r="C94" t="s">
-        <v>200</v>
-      </c>
-      <c r="D94" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A95" t="s">
-        <v>214</v>
-      </c>
-      <c r="B95">
-        <v>13</v>
-      </c>
-      <c r="C95" t="s">
-        <v>200</v>
-      </c>
-      <c r="D95" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A96" t="s">
-        <v>215</v>
-      </c>
-      <c r="B96">
-        <v>14</v>
-      </c>
-      <c r="C96" t="s">
-        <v>200</v>
-      </c>
-      <c r="D96" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A97" t="s">
-        <v>216</v>
-      </c>
-      <c r="B97">
-        <v>15</v>
-      </c>
-      <c r="C97" t="s">
-        <v>200</v>
-      </c>
-      <c r="D97" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98" t="s">
-        <v>217</v>
-      </c>
-      <c r="B98">
-        <v>16</v>
-      </c>
-      <c r="C98" t="s">
-        <v>200</v>
-      </c>
-      <c r="D98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A99" t="s">
-        <v>218</v>
-      </c>
-      <c r="B99">
-        <v>17</v>
-      </c>
-      <c r="C99" t="s">
-        <v>200</v>
-      </c>
-      <c r="D99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A100" t="s">
-        <v>219</v>
-      </c>
-      <c r="B100">
-        <v>18</v>
-      </c>
-      <c r="C100" t="s">
-        <v>200</v>
-      </c>
-      <c r="D100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A101" t="s">
-        <v>220</v>
-      </c>
-      <c r="B101">
-        <v>19</v>
-      </c>
-      <c r="C101" t="s">
-        <v>200</v>
-      </c>
-      <c r="D101" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A102" t="s">
-        <v>221</v>
-      </c>
-      <c r="B102">
+      <c r="B102" s="2">
         <v>20</v>
       </c>
       <c r="C102" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D102" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A103" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" t="s">
@@ -2554,11 +3202,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A104" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C104" t="s">
@@ -2568,11 +3216,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A105" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C105" t="s">
@@ -2582,11 +3230,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A106" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C106" t="s">
@@ -2596,11 +3244,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A107" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C107" t="s">
@@ -2610,11 +3258,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A108" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C108" t="s">
@@ -2624,11 +3272,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A109" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C109" t="s">
@@ -2638,11 +3286,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A110" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C110" t="s">
@@ -2652,11 +3300,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A111" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C111" t="s">
@@ -2666,11 +3314,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A112" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C112" t="s">
@@ -2680,11 +3328,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A113" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C113" t="s">
@@ -2694,11 +3342,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A114" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C114" t="s">
@@ -2708,11 +3356,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A115" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C115" t="s">
@@ -2722,11 +3370,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A116" t="s">
-        <v>125</v>
-      </c>
-      <c r="B116" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C116" t="s">
@@ -2736,11 +3384,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A117" t="s">
-        <v>134</v>
-      </c>
-      <c r="B117" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C117" t="s">
@@ -2750,11 +3398,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A118" t="s">
-        <v>138</v>
-      </c>
-      <c r="B118" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C118" t="s">
@@ -2764,11 +3412,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A119" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C119" t="s">
@@ -2778,11 +3426,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A120" t="s">
-        <v>144</v>
-      </c>
-      <c r="B120" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C120" t="s">
@@ -2792,11 +3440,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A121" t="s">
-        <v>151</v>
-      </c>
-      <c r="B121" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C121" t="s">
@@ -2804,6 +3452,1504 @@
       </c>
       <c r="D121" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"added Focus and minor voci corrections"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACE48370-6587-4EEA-A60C-EC1EEDE5AC97}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E086023B-DC06-453D-A9F0-3A0345269CDD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$C$261</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$C$260</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="508">
   <si>
     <t>Griechisch</t>
   </si>
@@ -878,12 +878,6 @@
     <t>bevorzugen</t>
   </si>
   <si>
-    <t>η φοιτήτρια</t>
-  </si>
-  <si>
-    <t>die Studentin</t>
-  </si>
-  <si>
     <t>γιατί</t>
   </si>
   <si>
@@ -1133,15 +1127,9 @@
     <t>die Freundin</t>
   </si>
   <si>
-    <t>αύπιο</t>
-  </si>
-  <si>
     <t>morgen</t>
   </si>
   <si>
-    <t>από αύπιο</t>
-  </si>
-  <si>
     <t>ab morgen</t>
   </si>
   <si>
@@ -1569,6 +1557,12 @@
   </si>
   <si>
     <t>τα κινέζικα</t>
+  </si>
+  <si>
+    <t>αύριο</t>
+  </si>
+  <si>
+    <t>από αύριο</t>
   </si>
 </sst>
 </file>
@@ -1944,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
-  <dimension ref="A1:D261"/>
+  <dimension ref="A1:D260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C218" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2181,7 +2175,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
@@ -2201,7 +2195,7 @@
         <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -2215,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -2229,7 +2223,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -2243,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -2257,7 +2251,7 @@
         <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -2271,7 +2265,7 @@
         <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -3651,10 +3645,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B122" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C122" t="s">
         <v>50</v>
@@ -3665,10 +3659,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B123" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C123" t="s">
         <v>50</v>
@@ -3679,10 +3673,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B124" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C124" t="s">
         <v>7</v>
@@ -3889,7 +3883,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B139" t="s">
         <v>274</v>
@@ -3903,10 +3897,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B140" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -3917,10 +3911,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B141" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C141" t="s">
         <v>7</v>
@@ -3931,10 +3925,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>279</v>
+        <v>424</v>
       </c>
       <c r="B142" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C142" t="s">
         <v>7</v>
@@ -3945,7 +3939,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>428</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
         <v>287</v>
@@ -3973,10 +3967,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>290</v>
+        <v>425</v>
       </c>
       <c r="B145" t="s">
-        <v>291</v>
+        <v>433</v>
       </c>
       <c r="C145" t="s">
         <v>7</v>
@@ -3987,10 +3981,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="B146" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C146" t="s">
         <v>7</v>
@@ -4001,10 +3995,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="B147" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -4015,10 +4009,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>455</v>
+        <v>294</v>
       </c>
       <c r="B148" t="s">
-        <v>454</v>
+        <v>295</v>
       </c>
       <c r="C148" t="s">
         <v>7</v>
@@ -4029,10 +4023,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B149" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C149" t="s">
         <v>7</v>
@@ -4071,10 +4065,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B152" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="C152" t="s">
         <v>7</v>
@@ -4099,10 +4093,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>322</v>
+        <v>439</v>
       </c>
       <c r="B154" t="s">
-        <v>323</v>
+        <v>441</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
@@ -4113,10 +4107,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B155" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C155" t="s">
         <v>7</v>
@@ -4127,10 +4121,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>442</v>
+        <v>326</v>
       </c>
       <c r="B156" t="s">
-        <v>444</v>
+        <v>327</v>
       </c>
       <c r="C156" t="s">
         <v>7</v>
@@ -4141,10 +4135,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B157" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C157" t="s">
         <v>7</v>
@@ -4155,10 +4149,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="B158" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="C158" t="s">
         <v>7</v>
@@ -4169,10 +4163,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="B159" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -4183,10 +4177,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B160" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C160" t="s">
         <v>7</v>
@@ -4197,10 +4191,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B161" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="C161" t="s">
         <v>7</v>
@@ -4211,10 +4205,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>370</v>
+        <v>478</v>
       </c>
       <c r="B162" t="s">
-        <v>371</v>
+        <v>452</v>
       </c>
       <c r="C162" t="s">
         <v>7</v>
@@ -4225,10 +4219,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>482</v>
+        <v>368</v>
       </c>
       <c r="B163" t="s">
-        <v>456</v>
+        <v>369</v>
       </c>
       <c r="C163" t="s">
         <v>7</v>
@@ -4239,10 +4233,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>372</v>
+        <v>479</v>
       </c>
       <c r="B164" t="s">
-        <v>373</v>
+        <v>453</v>
       </c>
       <c r="C164" t="s">
         <v>7</v>
@@ -4253,10 +4247,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>483</v>
+        <v>298</v>
       </c>
       <c r="B165" t="s">
-        <v>457</v>
+        <v>299</v>
       </c>
       <c r="C165" t="s">
         <v>7</v>
@@ -4267,10 +4261,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>300</v>
+        <v>480</v>
       </c>
       <c r="B166" t="s">
-        <v>301</v>
+        <v>454</v>
       </c>
       <c r="C166" t="s">
         <v>7</v>
@@ -4281,10 +4275,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B167" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C167" t="s">
         <v>7</v>
@@ -4295,10 +4289,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B168" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C168" t="s">
         <v>7</v>
@@ -4309,10 +4303,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B169" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C169" t="s">
         <v>7</v>
@@ -4323,10 +4317,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B170" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C170" t="s">
         <v>7</v>
@@ -4337,10 +4331,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B171" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C171" t="s">
         <v>7</v>
@@ -4351,10 +4345,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B172" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C172" t="s">
         <v>7</v>
@@ -4365,10 +4359,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B173" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C173" t="s">
         <v>7</v>
@@ -4379,10 +4373,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B174" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C174" t="s">
         <v>7</v>
@@ -4393,10 +4387,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B175" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C175" t="s">
         <v>7</v>
@@ -4407,10 +4401,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B176" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C176" t="s">
         <v>7</v>
@@ -4421,10 +4415,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B177" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C177" t="s">
         <v>7</v>
@@ -4435,10 +4429,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B178" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C178" t="s">
         <v>7</v>
@@ -4449,10 +4443,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B179" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C179" t="s">
         <v>7</v>
@@ -4463,10 +4457,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B180" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C180" t="s">
         <v>7</v>
@@ -4477,10 +4471,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>498</v>
+        <v>436</v>
       </c>
       <c r="B181" t="s">
-        <v>472</v>
+        <v>437</v>
       </c>
       <c r="C181" t="s">
         <v>7</v>
@@ -4491,10 +4485,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>440</v>
+        <v>376</v>
       </c>
       <c r="B182" t="s">
-        <v>441</v>
+        <v>377</v>
       </c>
       <c r="C182" t="s">
         <v>7</v>
@@ -4505,10 +4499,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B183" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C183" t="s">
         <v>7</v>
@@ -4519,10 +4513,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B184" t="s">
-        <v>383</v>
+        <v>426</v>
       </c>
       <c r="C184" t="s">
         <v>7</v>
@@ -4533,10 +4527,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B185" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="C185" t="s">
         <v>7</v>
@@ -4561,10 +4555,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B187" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C187" t="s">
         <v>7</v>
@@ -4575,10 +4569,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B188" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C188" t="s">
         <v>7</v>
@@ -4589,10 +4583,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B189" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C189" t="s">
         <v>7</v>
@@ -4603,10 +4597,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B190" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C190" t="s">
         <v>7</v>
@@ -4617,10 +4611,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B191" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C191" t="s">
         <v>7</v>
@@ -4659,10 +4653,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B194" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C194" t="s">
         <v>7</v>
@@ -4673,10 +4667,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B195" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C195" t="s">
         <v>7</v>
@@ -4701,13 +4695,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>425</v>
+        <v>306</v>
       </c>
       <c r="B197" t="s">
-        <v>426</v>
+        <v>307</v>
       </c>
       <c r="C197" t="s">
-        <v>7</v>
+        <v>445</v>
       </c>
       <c r="D197" t="s">
         <v>230</v>
@@ -4715,13 +4709,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B198" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C198" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D198" t="s">
         <v>230</v>
@@ -4729,13 +4723,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B199" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C199" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D199" t="s">
         <v>230</v>
@@ -4743,13 +4737,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>316</v>
+        <v>496</v>
       </c>
       <c r="B200" t="s">
-        <v>317</v>
+        <v>495</v>
       </c>
       <c r="C200" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D200" t="s">
         <v>230</v>
@@ -4757,13 +4751,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B201" t="s">
-        <v>499</v>
+        <v>469</v>
       </c>
       <c r="C201" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D201" t="s">
         <v>230</v>
@@ -4771,13 +4765,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B202" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C202" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D202" t="s">
         <v>230</v>
@@ -4785,13 +4779,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B203" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C203" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D203" t="s">
         <v>230</v>
@@ -4799,13 +4793,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B204" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C204" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D204" t="s">
         <v>230</v>
@@ -4813,13 +4807,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B205" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C205" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D205" t="s">
         <v>230</v>
@@ -4827,13 +4821,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B206" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C206" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D206" t="s">
         <v>230</v>
@@ -4841,13 +4835,13 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B207" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C207" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D207" t="s">
         <v>230</v>
@@ -4855,13 +4849,13 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B208" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C208" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D208" t="s">
         <v>230</v>
@@ -4869,13 +4863,13 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B209" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C209" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D209" t="s">
         <v>230</v>
@@ -4883,13 +4877,13 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>509</v>
+        <v>372</v>
       </c>
       <c r="B210" t="s">
-        <v>481</v>
+        <v>373</v>
       </c>
       <c r="C210" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D210" t="s">
         <v>230</v>
@@ -4897,13 +4891,13 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B211" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C211" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D211" t="s">
         <v>230</v>
@@ -4911,13 +4905,13 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>378</v>
+        <v>427</v>
       </c>
       <c r="B212" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C212" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D212" t="s">
         <v>230</v>
@@ -4925,13 +4919,13 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>431</v>
+        <v>346</v>
       </c>
       <c r="B213" t="s">
-        <v>233</v>
+        <v>347</v>
       </c>
       <c r="C213" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D213" t="s">
         <v>230</v>
@@ -4939,13 +4933,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>348</v>
+        <v>428</v>
       </c>
       <c r="B214" t="s">
-        <v>349</v>
+        <v>238</v>
       </c>
       <c r="C214" t="s">
-        <v>449</v>
+        <v>26</v>
       </c>
       <c r="D214" t="s">
         <v>230</v>
@@ -4953,10 +4947,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>432</v>
+        <v>251</v>
       </c>
       <c r="B215" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="C215" t="s">
         <v>26</v>
@@ -4967,10 +4961,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="B216" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="C216" t="s">
         <v>26</v>
@@ -4981,10 +4975,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="B217" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="C217" t="s">
         <v>26</v>
@@ -4995,10 +4989,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="B218" t="s">
-        <v>295</v>
+        <v>323</v>
       </c>
       <c r="C218" t="s">
         <v>26</v>
@@ -5009,10 +5003,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B219" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C219" t="s">
         <v>26</v>
@@ -5023,10 +5017,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B220" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C220" t="s">
         <v>26</v>
@@ -5037,10 +5031,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B221" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C221" t="s">
         <v>26</v>
@@ -5051,10 +5045,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B222" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="C222" t="s">
         <v>26</v>
@@ -5079,10 +5073,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>354</v>
+        <v>506</v>
       </c>
       <c r="B224" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="C224" t="s">
         <v>26</v>
@@ -5093,10 +5087,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>364</v>
+        <v>507</v>
       </c>
       <c r="B225" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C225" t="s">
         <v>26</v>
@@ -5107,10 +5101,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>366</v>
+        <v>419</v>
       </c>
       <c r="B226" t="s">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="C226" t="s">
         <v>26</v>
@@ -5121,13 +5115,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>423</v>
+        <v>247</v>
       </c>
       <c r="B227" t="s">
-        <v>424</v>
+        <v>248</v>
       </c>
       <c r="C227" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D227" t="s">
         <v>230</v>
@@ -5135,10 +5129,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="B228" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="C228" t="s">
         <v>13</v>
@@ -5149,10 +5143,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="B229" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="C229" t="s">
         <v>13</v>
@@ -5163,10 +5157,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="B230" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="C230" t="s">
         <v>13</v>
@@ -5177,13 +5171,13 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="B231" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="C231" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D231" t="s">
         <v>230</v>
@@ -5191,10 +5185,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>275</v>
+        <v>364</v>
       </c>
       <c r="B232" t="s">
-        <v>276</v>
+        <v>365</v>
       </c>
       <c r="C232" t="s">
         <v>11</v>
@@ -5205,10 +5199,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B233" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C233" t="s">
         <v>11</v>
@@ -5219,10 +5213,10 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="B234" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="C234" t="s">
         <v>11</v>
@@ -5233,10 +5227,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B235" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C235" t="s">
         <v>11</v>
@@ -5247,10 +5241,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="B236" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="C236" t="s">
         <v>11</v>
@@ -5261,10 +5255,10 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>405</v>
+        <v>448</v>
       </c>
       <c r="B237" t="s">
-        <v>406</v>
+        <v>446</v>
       </c>
       <c r="C237" t="s">
         <v>11</v>
@@ -5275,10 +5269,10 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B238" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C238" t="s">
         <v>11</v>
@@ -5289,13 +5283,13 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>453</v>
+        <v>243</v>
       </c>
       <c r="B239" t="s">
-        <v>451</v>
+        <v>244</v>
       </c>
       <c r="C239" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D239" t="s">
         <v>230</v>
@@ -5303,10 +5297,10 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B240" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C240" t="s">
         <v>6</v>
@@ -5317,10 +5311,10 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B241" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C241" t="s">
         <v>6</v>
@@ -5331,10 +5325,10 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="B242" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="C242" t="s">
         <v>6</v>
@@ -5345,10 +5339,10 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="B243" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="C243" t="s">
         <v>6</v>
@@ -5359,10 +5353,10 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B244" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C244" t="s">
         <v>6</v>
@@ -5387,10 +5381,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B246" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C246" t="s">
         <v>6</v>
@@ -5401,10 +5395,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="B247" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="C247" t="s">
         <v>6</v>
@@ -5415,10 +5409,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B248" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="C248" t="s">
         <v>6</v>
@@ -5429,10 +5423,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B249" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C249" t="s">
         <v>6</v>
@@ -5443,10 +5437,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B250" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C250" t="s">
         <v>6</v>
@@ -5457,10 +5451,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B251" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C251" t="s">
         <v>6</v>
@@ -5471,10 +5465,10 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B252" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="C252" t="s">
         <v>6</v>
@@ -5485,10 +5479,10 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B253" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C253" t="s">
         <v>6</v>
@@ -5499,10 +5493,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B254" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C254" t="s">
         <v>6</v>
@@ -5513,10 +5507,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B255" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C255" t="s">
         <v>6</v>
@@ -5527,10 +5521,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="B256" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="C256" t="s">
         <v>6</v>
@@ -5555,10 +5549,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="B258" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
       <c r="C258" t="s">
         <v>6</v>
@@ -5583,37 +5577,23 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="B260" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="C260" t="s">
-        <v>6</v>
+        <v>197</v>
       </c>
       <c r="D260" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A261" t="s">
-        <v>407</v>
-      </c>
-      <c r="B261" t="s">
-        <v>408</v>
-      </c>
-      <c r="C261" t="s">
-        <v>197</v>
-      </c>
-      <c r="D261" t="s">
-        <v>230</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="C1:C261" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D261">
-    <sortCondition ref="D1:D261"/>
-    <sortCondition ref="C1:C261"/>
+  <autoFilter ref="C1:C260" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D260">
+    <sortCondition ref="D1:D260"/>
+    <sortCondition ref="C1:C260"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"changed setup to SQL"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E086023B-DC06-453D-A9F0-3A0345269CDD}"/>
+  <xr:revisionPtr revIDLastSave="332" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{189CE10C-8788-4B18-BDD1-DAC37956A2FB}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$C$260</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="506">
   <si>
     <t>Griechisch</t>
   </si>
   <si>
     <t>Deutsch</t>
-  </si>
-  <si>
-    <t>Kategorie</t>
-  </si>
-  <si>
-    <t>Typ</t>
   </si>
   <si>
     <t>Lehrbuch 1</t>
@@ -1938,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
-  <dimension ref="A1:D260"/>
+  <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C218" sqref="C218"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1951,13 +1942,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1965,100 +1956,100 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2069,24 +2060,24 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -2097,220 +2088,220 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>440</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>442</v>
+        <v>126</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>443</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>445</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>220</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -2321,66 +2312,66 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
         <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -2391,598 +2382,598 @@
         <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B46" t="s">
-        <v>213</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>212</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="B61" t="s">
-        <v>215</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>180</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>181</v>
+        <v>33</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>181</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
       <c r="B66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>188</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s">
-        <v>185</v>
+        <v>53</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>216</v>
       </c>
       <c r="B68" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="B69" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B70" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>187</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="B73" t="s">
         <v>49</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="C74" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -2993,192 +2984,192 @@
         <v>176</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="B77" t="s">
-        <v>62</v>
+        <v>215</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B78" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>193</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D84" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B88" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
@@ -3189,10 +3180,10 @@
         <v>37</v>
       </c>
       <c r="C89" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D89" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
@@ -3203,10 +3194,10 @@
         <v>39</v>
       </c>
       <c r="C90" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
@@ -3217,10 +3208,10 @@
         <v>41</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
@@ -3231,486 +3222,486 @@
         <v>43</v>
       </c>
       <c r="C92" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C93" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B94" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B95" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B96" t="s">
         <v>64</v>
       </c>
       <c r="C96" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B99" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D99" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>149</v>
-      </c>
-      <c r="B100" t="s">
-        <v>79</v>
+        <v>196</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="D100" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D101" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C102" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D102" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D103" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D105" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D106" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="B107">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D107" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B108">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D108" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B109">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D109" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B110">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D110" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="B111">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C111" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D111" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B112">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C112" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D112" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B113">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C113" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D113" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B114">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C114" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D114" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B115">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C115" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D115" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B116">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C116" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D116" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B117">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C117" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D117" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B118">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C118" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D118" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B119">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C119" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D119" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B120">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C120" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D120" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>212</v>
-      </c>
-      <c r="B121">
-        <v>20</v>
+        <v>310</v>
+      </c>
+      <c r="B121" t="s">
+        <v>311</v>
       </c>
       <c r="C121" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
       <c r="D121" t="s">
-        <v>4</v>
+        <v>228</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>312</v>
+        <v>336</v>
       </c>
       <c r="B122" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="C122" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D122" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>338</v>
+        <v>441</v>
       </c>
       <c r="B123" t="s">
-        <v>339</v>
+        <v>442</v>
       </c>
       <c r="C123" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D123" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>443</v>
+        <v>226</v>
       </c>
       <c r="B124" t="s">
-        <v>444</v>
+        <v>227</v>
       </c>
       <c r="C124" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D124" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B125" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C125" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D125" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C126" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D126" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
@@ -3721,24 +3712,24 @@
         <v>235</v>
       </c>
       <c r="C127" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B128" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C128" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
@@ -3749,38 +3740,38 @@
         <v>240</v>
       </c>
       <c r="C129" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D129" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B130" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C130" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D130" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B131" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C131" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D131" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
@@ -3791,10 +3782,10 @@
         <v>256</v>
       </c>
       <c r="C132" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D132" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
@@ -3805,38 +3796,38 @@
         <v>258</v>
       </c>
       <c r="C133" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D133" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>82</v>
+      </c>
+      <c r="B134" t="s">
         <v>259</v>
       </c>
-      <c r="B134" t="s">
-        <v>260</v>
-      </c>
       <c r="C134" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D134" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>84</v>
+        <v>264</v>
       </c>
       <c r="B135" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C135" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D135" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
@@ -3847,94 +3838,94 @@
         <v>267</v>
       </c>
       <c r="C136" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D136" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B137" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C137" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D137" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>427</v>
+      </c>
+      <c r="B138" t="s">
         <v>272</v>
       </c>
-      <c r="B138" t="s">
-        <v>273</v>
-      </c>
       <c r="C138" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D138" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>428</v>
+      </c>
+      <c r="B139" t="s">
         <v>429</v>
       </c>
-      <c r="B139" t="s">
-        <v>274</v>
-      </c>
       <c r="C139" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D139" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>421</v>
+      </c>
+      <c r="B140" t="s">
         <v>430</v>
       </c>
-      <c r="B140" t="s">
-        <v>431</v>
-      </c>
       <c r="C140" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D140" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B141" t="s">
-        <v>432</v>
+        <v>283</v>
       </c>
       <c r="C141" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D141" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>424</v>
+        <v>284</v>
       </c>
       <c r="B142" t="s">
         <v>285</v>
       </c>
       <c r="C142" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D142" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
@@ -3945,80 +3936,80 @@
         <v>287</v>
       </c>
       <c r="C143" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D143" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>288</v>
+        <v>423</v>
       </c>
       <c r="B144" t="s">
-        <v>289</v>
+        <v>431</v>
       </c>
       <c r="C144" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D144" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="B145" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C145" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D145" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="B146" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="C146" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D146" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>451</v>
+        <v>292</v>
       </c>
       <c r="B147" t="s">
-        <v>450</v>
+        <v>293</v>
       </c>
       <c r="C147" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D147" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B148" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C148" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D148" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
@@ -4029,10 +4020,10 @@
         <v>301</v>
       </c>
       <c r="C149" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D149" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
@@ -4043,24 +4034,24 @@
         <v>303</v>
       </c>
       <c r="C150" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D150" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="B151" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="C151" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
@@ -4071,192 +4062,192 @@
         <v>319</v>
       </c>
       <c r="C152" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D152" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>320</v>
+        <v>437</v>
       </c>
       <c r="B153" t="s">
-        <v>321</v>
+        <v>439</v>
       </c>
       <c r="C153" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D153" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B154" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C154" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D154" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>438</v>
+        <v>324</v>
       </c>
       <c r="B155" t="s">
-        <v>440</v>
+        <v>325</v>
       </c>
       <c r="C155" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D155" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B156" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C156" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D156" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="B157" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C157" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D157" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="B158" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="C158" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D158" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B159" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C159" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D159" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B160" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C160" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D160" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>366</v>
+        <v>476</v>
       </c>
       <c r="B161" t="s">
-        <v>367</v>
+        <v>450</v>
       </c>
       <c r="C161" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D161" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>478</v>
+        <v>366</v>
       </c>
       <c r="B162" t="s">
-        <v>452</v>
+        <v>367</v>
       </c>
       <c r="C162" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D162" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>368</v>
+        <v>477</v>
       </c>
       <c r="B163" t="s">
-        <v>369</v>
+        <v>451</v>
       </c>
       <c r="C163" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D163" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>479</v>
+        <v>296</v>
       </c>
       <c r="B164" t="s">
-        <v>453</v>
+        <v>297</v>
       </c>
       <c r="C164" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D164" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>298</v>
+        <v>478</v>
       </c>
       <c r="B165" t="s">
-        <v>299</v>
+        <v>452</v>
       </c>
       <c r="C165" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D165" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
@@ -4264,27 +4255,27 @@
         <v>480</v>
       </c>
       <c r="B166" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C166" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D166" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B167" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C167" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D167" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
@@ -4292,195 +4283,195 @@
         <v>481</v>
       </c>
       <c r="B168" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C168" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B169" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C169" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D169" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B170" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C170" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D170" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B171" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C171" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D171" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B172" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C172" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D172" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B173" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C173" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D173" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B174" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C174" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D174" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B175" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C175" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D175" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B176" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C176" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D176" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B177" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C177" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D177" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B178" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C178" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D178" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B179" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C179" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D179" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>494</v>
+        <v>434</v>
       </c>
       <c r="B180" t="s">
-        <v>468</v>
+        <v>435</v>
       </c>
       <c r="C180" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D180" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>436</v>
+        <v>374</v>
       </c>
       <c r="B181" t="s">
-        <v>437</v>
+        <v>375</v>
       </c>
       <c r="C181" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D181" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
@@ -4491,10 +4482,10 @@
         <v>377</v>
       </c>
       <c r="C182" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D182" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
@@ -4502,41 +4493,41 @@
         <v>378</v>
       </c>
       <c r="B183" t="s">
-        <v>379</v>
+        <v>424</v>
       </c>
       <c r="C183" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D183" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="B184" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="C184" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D184" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B185" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C185" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D185" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
@@ -4547,10 +4538,10 @@
         <v>392</v>
       </c>
       <c r="C186" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D186" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
@@ -4561,10 +4552,10 @@
         <v>394</v>
       </c>
       <c r="C187" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D187" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
@@ -4575,10 +4566,10 @@
         <v>396</v>
       </c>
       <c r="C188" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D188" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
@@ -4589,52 +4580,52 @@
         <v>398</v>
       </c>
       <c r="C189" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D189" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B190" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C190" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D190" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B191" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C191" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D191" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B192" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C192" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D192" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
@@ -4645,10 +4636,10 @@
         <v>414</v>
       </c>
       <c r="C193" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D193" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
@@ -4659,220 +4650,220 @@
         <v>416</v>
       </c>
       <c r="C194" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D194" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B195" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C195" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D195" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>421</v>
+        <v>304</v>
       </c>
       <c r="B196" t="s">
-        <v>422</v>
+        <v>305</v>
       </c>
       <c r="C196" t="s">
-        <v>7</v>
+        <v>443</v>
       </c>
       <c r="D196" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B197" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C197" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D197" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B198" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C198" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D198" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>314</v>
+        <v>494</v>
       </c>
       <c r="B199" t="s">
-        <v>315</v>
+        <v>493</v>
       </c>
       <c r="C199" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D199" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B200" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="C200" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D200" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B201" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C201" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D201" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B202" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C202" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D202" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B203" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C203" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D203" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B204" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C204" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D204" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B205" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C205" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D205" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B206" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C206" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D206" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B207" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C207" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D207" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B208" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C208" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D208" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>505</v>
+        <v>370</v>
       </c>
       <c r="B209" t="s">
-        <v>477</v>
+        <v>371</v>
       </c>
       <c r="C209" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D209" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
@@ -4883,164 +4874,164 @@
         <v>373</v>
       </c>
       <c r="C210" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D210" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>374</v>
+        <v>425</v>
       </c>
       <c r="B211" t="s">
-        <v>375</v>
+        <v>231</v>
       </c>
       <c r="C211" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D211" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>427</v>
+        <v>344</v>
       </c>
       <c r="B212" t="s">
-        <v>233</v>
+        <v>345</v>
       </c>
       <c r="C212" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D212" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>346</v>
+        <v>426</v>
       </c>
       <c r="B213" t="s">
-        <v>347</v>
+        <v>236</v>
       </c>
       <c r="C213" t="s">
-        <v>445</v>
+        <v>24</v>
       </c>
       <c r="D213" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>428</v>
+        <v>249</v>
       </c>
       <c r="B214" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="C214" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D214" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="B215" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="C215" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D215" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B216" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="C216" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D216" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="B217" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="C217" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D217" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="B218" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="C218" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D218" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B219" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C219" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D219" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B220" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C220" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D220" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B221" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C221" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D221" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
@@ -5051,304 +5042,304 @@
         <v>351</v>
       </c>
       <c r="C222" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D222" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>352</v>
+        <v>504</v>
       </c>
       <c r="B223" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C223" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D223" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B224" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C224" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D224" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>507</v>
+        <v>417</v>
       </c>
       <c r="B225" t="s">
-        <v>363</v>
+        <v>418</v>
       </c>
       <c r="C225" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D225" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>419</v>
+        <v>245</v>
       </c>
       <c r="B226" t="s">
-        <v>420</v>
+        <v>246</v>
       </c>
       <c r="C226" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D226" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="B227" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="C227" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D227" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="B228" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="C228" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D228" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="B229" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="C229" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D229" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="B230" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="C230" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D230" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>275</v>
+        <v>362</v>
       </c>
       <c r="B231" t="s">
-        <v>276</v>
+        <v>363</v>
       </c>
       <c r="C231" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D231" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B232" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C232" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D232" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="B233" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="C233" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D233" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B234" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C234" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D234" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="B235" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C235" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D235" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>401</v>
+        <v>446</v>
       </c>
       <c r="B236" t="s">
-        <v>402</v>
+        <v>444</v>
       </c>
       <c r="C236" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D236" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B237" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C237" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D237" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>449</v>
+        <v>241</v>
       </c>
       <c r="B238" t="s">
-        <v>447</v>
+        <v>242</v>
       </c>
       <c r="C238" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D238" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B239" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C239" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D239" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B240" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C240" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D240" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="B241" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C241" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D241" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="B242" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C242" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D242" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B243" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C243" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D243" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
@@ -5359,241 +5350,226 @@
         <v>282</v>
       </c>
       <c r="C244" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D244" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B245" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C245" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D245" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="B246" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="C246" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D246" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B247" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C247" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D247" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B248" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C248" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D248" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B249" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C249" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D249" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B250" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="C250" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D250" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="B251" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="C251" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D251" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B252" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C252" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D252" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B253" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C253" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D253" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B254" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C254" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D254" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>358</v>
+        <v>379</v>
       </c>
       <c r="B255" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="C255" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D255" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B256" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C256" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D256" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="B257" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
       <c r="C257" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D257" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B258" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C258" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D258" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="B259" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="C259" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="D259" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A260" t="s">
-        <v>403</v>
-      </c>
-      <c r="B260" t="s">
-        <v>404</v>
-      </c>
-      <c r="C260" t="s">
-        <v>197</v>
-      </c>
-      <c r="D260" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C260" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D260">
-    <sortCondition ref="D1:D260"/>
-    <sortCondition ref="C1:C260"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D259">
+    <sortCondition ref="D1:D259"/>
+    <sortCondition ref="C1:C259"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"added Voci 4 #2"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="894" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84437411-568B-4CC0-9FF5-849339F8A0BC}"/>
+  <xr:revisionPtr revIDLastSave="933" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F00E455-6F68-4C34-9351-4BE18A0943DA}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="938">
   <si>
     <t>Griechisch</t>
   </si>
@@ -2759,9 +2759,6 @@
     <t>το διαζύγιο</t>
   </si>
   <si>
-    <t>die Verwanten</t>
-  </si>
-  <si>
     <t>die Eltern</t>
   </si>
   <si>
@@ -2787,6 +2784,72 @@
   </si>
   <si>
     <t>die Schweidung</t>
+  </si>
+  <si>
+    <t>Lehrbuch 4</t>
+  </si>
+  <si>
+    <t>die Verwandten</t>
+  </si>
+  <si>
+    <t>der Mann</t>
+  </si>
+  <si>
+    <t>der Ehemann</t>
+  </si>
+  <si>
+    <t>ledig</t>
+  </si>
+  <si>
+    <t>der Verlobte</t>
+  </si>
+  <si>
+    <t>die Verlobte</t>
+  </si>
+  <si>
+    <t>getrennt</t>
+  </si>
+  <si>
+    <t>geschieden</t>
+  </si>
+  <si>
+    <t>ο άντρας</t>
+  </si>
+  <si>
+    <t>ο σύζυγος</t>
+  </si>
+  <si>
+    <t>ανύπαντρος, ελεύθερος</t>
+  </si>
+  <si>
+    <t>ο αρραβωνιαστικός</t>
+  </si>
+  <si>
+    <t>η αρραβωνιαστικά</t>
+  </si>
+  <si>
+    <t>χωρισμένος</t>
+  </si>
+  <si>
+    <t>διαζευγμένος</t>
+  </si>
+  <si>
+    <t>die Witwe</t>
+  </si>
+  <si>
+    <t>der Witwer</t>
+  </si>
+  <si>
+    <t>ο χήρος</t>
+  </si>
+  <si>
+    <t>η χήρα</t>
+  </si>
+  <si>
+    <t>die Ehefrau</t>
+  </si>
+  <si>
+    <t>η σύζυγη</t>
   </si>
 </sst>
 </file>
@@ -3165,15 +3228,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
-  <dimension ref="A1:D470"/>
+  <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A450" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C471" sqref="C471"/>
+    <sheetView tabSelected="1" topLeftCell="A457" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D469" sqref="D469:D480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="18.1328125" customWidth="1"/>
+    <col min="1" max="1" width="20.796875" customWidth="1"/>
+    <col min="2" max="4" width="18.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -8716,6 +8780,9 @@
       <c r="C396" t="s">
         <v>5</v>
       </c>
+      <c r="D396" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
@@ -8727,6 +8794,9 @@
       <c r="C397" t="s">
         <v>5</v>
       </c>
+      <c r="D397" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
@@ -8738,6 +8808,9 @@
       <c r="C398" t="s">
         <v>5</v>
       </c>
+      <c r="D398" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
@@ -8749,6 +8822,9 @@
       <c r="C399" t="s">
         <v>5</v>
       </c>
+      <c r="D399" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
@@ -8760,8 +8836,11 @@
       <c r="C400" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D400" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>778</v>
       </c>
@@ -8771,8 +8850,11 @@
       <c r="C401" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D401" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>779</v>
       </c>
@@ -8782,8 +8864,11 @@
       <c r="C402" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D402" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>780</v>
       </c>
@@ -8793,8 +8878,11 @@
       <c r="C403" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D403" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>781</v>
       </c>
@@ -8804,8 +8892,11 @@
       <c r="C404" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D404" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>782</v>
       </c>
@@ -8815,8 +8906,11 @@
       <c r="C405" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D405" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>845</v>
       </c>
@@ -8826,8 +8920,11 @@
       <c r="C406" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D406" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>783</v>
       </c>
@@ -8837,8 +8934,11 @@
       <c r="C407" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D407" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>784</v>
       </c>
@@ -8848,8 +8948,11 @@
       <c r="C408" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D408" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>785</v>
       </c>
@@ -8859,8 +8962,11 @@
       <c r="C409" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D409" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>786</v>
       </c>
@@ -8870,8 +8976,11 @@
       <c r="C410" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D410" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>787</v>
       </c>
@@ -8881,8 +8990,11 @@
       <c r="C411" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D411" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>788</v>
       </c>
@@ -8892,8 +9004,11 @@
       <c r="C412" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D412" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>789</v>
       </c>
@@ -8903,8 +9018,11 @@
       <c r="C413" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D413" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>790</v>
       </c>
@@ -8914,8 +9032,11 @@
       <c r="C414" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D414" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>791</v>
       </c>
@@ -8925,8 +9046,11 @@
       <c r="C415" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D415" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>792</v>
       </c>
@@ -8936,8 +9060,11 @@
       <c r="C416" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D416" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>793</v>
       </c>
@@ -8947,8 +9074,11 @@
       <c r="C417" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D417" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>794</v>
       </c>
@@ -8958,8 +9088,11 @@
       <c r="C418" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D418" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>795</v>
       </c>
@@ -8969,8 +9102,11 @@
       <c r="C419" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D419" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>796</v>
       </c>
@@ -8980,8 +9116,11 @@
       <c r="C420" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D420" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>797</v>
       </c>
@@ -8991,8 +9130,11 @@
       <c r="C421" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D421" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>798</v>
       </c>
@@ -9002,8 +9144,11 @@
       <c r="C422" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D422" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>799</v>
       </c>
@@ -9013,8 +9158,11 @@
       <c r="C423" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D423" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>800</v>
       </c>
@@ -9024,8 +9172,11 @@
       <c r="C424" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D424" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>801</v>
       </c>
@@ -9035,8 +9186,11 @@
       <c r="C425" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D425" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>802</v>
       </c>
@@ -9046,8 +9200,11 @@
       <c r="C426" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D426" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>803</v>
       </c>
@@ -9057,8 +9214,11 @@
       <c r="C427" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D427" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>804</v>
       </c>
@@ -9068,8 +9228,11 @@
       <c r="C428" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D428" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
         <v>805</v>
       </c>
@@ -9079,8 +9242,11 @@
       <c r="C429" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D429" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
         <v>806</v>
       </c>
@@ -9090,8 +9256,11 @@
       <c r="C430" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D430" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
         <v>807</v>
       </c>
@@ -9101,8 +9270,11 @@
       <c r="C431" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D431" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
         <v>808</v>
       </c>
@@ -9112,8 +9284,11 @@
       <c r="C432" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D432" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
         <v>809</v>
       </c>
@@ -9123,8 +9298,11 @@
       <c r="C433" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D433" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
         <v>810</v>
       </c>
@@ -9134,8 +9312,11 @@
       <c r="C434" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D434" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
         <v>811</v>
       </c>
@@ -9145,8 +9326,11 @@
       <c r="C435" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D435" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
         <v>812</v>
       </c>
@@ -9156,8 +9340,11 @@
       <c r="C436" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D436" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
         <v>813</v>
       </c>
@@ -9167,8 +9354,11 @@
       <c r="C437" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D437" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
         <v>814</v>
       </c>
@@ -9178,8 +9368,11 @@
       <c r="C438" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D438" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
         <v>815</v>
       </c>
@@ -9189,8 +9382,11 @@
       <c r="C439" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D439" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
         <v>816</v>
       </c>
@@ -9200,8 +9396,11 @@
       <c r="C440" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D440" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
         <v>817</v>
       </c>
@@ -9211,8 +9410,11 @@
       <c r="C441" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D441" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
         <v>818</v>
       </c>
@@ -9222,8 +9424,11 @@
       <c r="C442" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D442" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
         <v>819</v>
       </c>
@@ -9233,8 +9438,11 @@
       <c r="C443" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D443" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
         <v>820</v>
       </c>
@@ -9244,8 +9452,11 @@
       <c r="C444" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D444" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
         <v>821</v>
       </c>
@@ -9255,8 +9466,11 @@
       <c r="C445" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D445" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
         <v>822</v>
       </c>
@@ -9266,8 +9480,11 @@
       <c r="C446" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D446" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
         <v>823</v>
       </c>
@@ -9277,8 +9494,11 @@
       <c r="C447" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="448" spans="1:3" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="D447" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A448" s="1" t="s">
         <v>884</v>
       </c>
@@ -9288,8 +9508,11 @@
       <c r="C448" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D448" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
         <v>824</v>
       </c>
@@ -9299,8 +9522,11 @@
       <c r="C449" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D449" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
         <v>825</v>
       </c>
@@ -9310,8 +9536,11 @@
       <c r="C450" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D450" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
         <v>826</v>
       </c>
@@ -9321,8 +9550,11 @@
       <c r="C451" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D451" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
         <v>827</v>
       </c>
@@ -9332,8 +9564,11 @@
       <c r="C452" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D452" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
         <v>828</v>
       </c>
@@ -9343,8 +9578,11 @@
       <c r="C453" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D453" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
         <v>829</v>
       </c>
@@ -9354,8 +9592,11 @@
       <c r="C454" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D454" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
         <v>830</v>
       </c>
@@ -9365,8 +9606,11 @@
       <c r="C455" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D455" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
         <v>831</v>
       </c>
@@ -9376,8 +9620,11 @@
       <c r="C456" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D456" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
         <v>832</v>
       </c>
@@ -9387,8 +9634,11 @@
       <c r="C457" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D457" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
         <v>833</v>
       </c>
@@ -9398,8 +9648,11 @@
       <c r="C458" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D458" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
         <v>834</v>
       </c>
@@ -9409,8 +9662,11 @@
       <c r="C459" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D459" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
         <v>895</v>
       </c>
@@ -9420,115 +9676,288 @@
       <c r="C460" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D460" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
         <v>897</v>
       </c>
       <c r="B461" t="s">
-        <v>907</v>
+        <v>917</v>
       </c>
       <c r="C461" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D461" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
         <v>898</v>
       </c>
       <c r="B462" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C462" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D462" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
         <v>899</v>
       </c>
       <c r="B463" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C463" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D463" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
         <v>900</v>
       </c>
       <c r="B464" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C464" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D464" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
         <v>901</v>
       </c>
       <c r="B465" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C465" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D465" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
         <v>902</v>
       </c>
       <c r="B466" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C466" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D466" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
         <v>903</v>
       </c>
       <c r="B467" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C467" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D467" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
         <v>904</v>
       </c>
       <c r="B468" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C468" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D468" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
         <v>905</v>
       </c>
       <c r="B469" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C469" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D469" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
         <v>906</v>
       </c>
       <c r="B470" t="s">
+        <v>915</v>
+      </c>
+      <c r="C470" t="s">
+        <v>5</v>
+      </c>
+      <c r="D470" t="s">
         <v>916</v>
       </c>
-      <c r="C470" t="s">
-        <v>5</v>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A471" t="s">
+        <v>925</v>
+      </c>
+      <c r="B471" t="s">
+        <v>918</v>
+      </c>
+      <c r="C471" t="s">
+        <v>5</v>
+      </c>
+      <c r="D471" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A472" t="s">
+        <v>926</v>
+      </c>
+      <c r="B472" t="s">
+        <v>919</v>
+      </c>
+      <c r="C472" t="s">
+        <v>5</v>
+      </c>
+      <c r="D472" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A473" t="s">
+        <v>927</v>
+      </c>
+      <c r="B473" t="s">
+        <v>920</v>
+      </c>
+      <c r="C473" t="s">
+        <v>48</v>
+      </c>
+      <c r="D473" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A474" t="s">
+        <v>928</v>
+      </c>
+      <c r="B474" t="s">
+        <v>921</v>
+      </c>
+      <c r="C474" t="s">
+        <v>5</v>
+      </c>
+      <c r="D474" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A475" t="s">
+        <v>929</v>
+      </c>
+      <c r="B475" t="s">
+        <v>922</v>
+      </c>
+      <c r="C475" t="s">
+        <v>5</v>
+      </c>
+      <c r="D475" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A476" t="s">
+        <v>930</v>
+      </c>
+      <c r="B476" t="s">
+        <v>923</v>
+      </c>
+      <c r="C476" t="s">
+        <v>48</v>
+      </c>
+      <c r="D476" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A477" t="s">
+        <v>931</v>
+      </c>
+      <c r="B477" t="s">
+        <v>924</v>
+      </c>
+      <c r="C477" t="s">
+        <v>48</v>
+      </c>
+      <c r="D477" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A478" t="s">
+        <v>934</v>
+      </c>
+      <c r="B478" t="s">
+        <v>933</v>
+      </c>
+      <c r="C478" t="s">
+        <v>5</v>
+      </c>
+      <c r="D478" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A479" t="s">
+        <v>935</v>
+      </c>
+      <c r="B479" t="s">
+        <v>932</v>
+      </c>
+      <c r="C479" t="s">
+        <v>5</v>
+      </c>
+      <c r="D479" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A480" t="s">
+        <v>937</v>
+      </c>
+      <c r="B480" t="s">
+        <v>936</v>
+      </c>
+      <c r="C480" t="s">
+        <v>5</v>
+      </c>
+      <c r="D480" t="s">
+        <v>916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"added delete sql function"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="933" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F00E455-6F68-4C34-9351-4BE18A0943DA}"/>
+  <xr:revisionPtr revIDLastSave="934" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE442FFF-5BD4-4F54-B523-CEF0A58C4B0B}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="11033" windowHeight="13763" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2783,9 +2783,6 @@
     <t>die Trennung</t>
   </si>
   <si>
-    <t>die Schweidung</t>
-  </si>
-  <si>
     <t>Lehrbuch 4</t>
   </si>
   <si>
@@ -2850,6 +2847,9 @@
   </si>
   <si>
     <t>η σύζυγη</t>
+  </si>
+  <si>
+    <t>die Scheidung</t>
   </si>
 </sst>
 </file>
@@ -3230,8 +3230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A457" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D469" sqref="D469:D480"/>
+    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C403" sqref="C403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -8781,7 +8781,7 @@
         <v>5</v>
       </c>
       <c r="D396" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.35">
@@ -8795,7 +8795,7 @@
         <v>5</v>
       </c>
       <c r="D397" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.35">
@@ -8809,7 +8809,7 @@
         <v>5</v>
       </c>
       <c r="D398" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.35">
@@ -8823,7 +8823,7 @@
         <v>5</v>
       </c>
       <c r="D399" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.35">
@@ -8837,7 +8837,7 @@
         <v>5</v>
       </c>
       <c r="D400" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.35">
@@ -8851,7 +8851,7 @@
         <v>5</v>
       </c>
       <c r="D401" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.35">
@@ -8865,7 +8865,7 @@
         <v>5</v>
       </c>
       <c r="D402" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.35">
@@ -8879,7 +8879,7 @@
         <v>5</v>
       </c>
       <c r="D403" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.35">
@@ -8893,7 +8893,7 @@
         <v>5</v>
       </c>
       <c r="D404" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.35">
@@ -8907,7 +8907,7 @@
         <v>5</v>
       </c>
       <c r="D405" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.35">
@@ -8921,7 +8921,7 @@
         <v>5</v>
       </c>
       <c r="D406" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.35">
@@ -8935,7 +8935,7 @@
         <v>5</v>
       </c>
       <c r="D407" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.35">
@@ -8949,7 +8949,7 @@
         <v>48</v>
       </c>
       <c r="D408" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.35">
@@ -8963,7 +8963,7 @@
         <v>5</v>
       </c>
       <c r="D409" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.35">
@@ -8977,7 +8977,7 @@
         <v>11</v>
       </c>
       <c r="D410" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.35">
@@ -8991,7 +8991,7 @@
         <v>5</v>
       </c>
       <c r="D411" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.35">
@@ -9005,7 +9005,7 @@
         <v>24</v>
       </c>
       <c r="D412" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.35">
@@ -9019,7 +9019,7 @@
         <v>5</v>
       </c>
       <c r="D413" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.35">
@@ -9033,7 +9033,7 @@
         <v>5</v>
       </c>
       <c r="D414" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.35">
@@ -9047,7 +9047,7 @@
         <v>11</v>
       </c>
       <c r="D415" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.35">
@@ -9061,7 +9061,7 @@
         <v>48</v>
       </c>
       <c r="D416" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.35">
@@ -9075,7 +9075,7 @@
         <v>5</v>
       </c>
       <c r="D417" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.35">
@@ -9089,7 +9089,7 @@
         <v>48</v>
       </c>
       <c r="D418" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.35">
@@ -9103,7 +9103,7 @@
         <v>5</v>
       </c>
       <c r="D419" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.35">
@@ -9117,7 +9117,7 @@
         <v>48</v>
       </c>
       <c r="D420" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.35">
@@ -9131,7 +9131,7 @@
         <v>48</v>
       </c>
       <c r="D421" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.35">
@@ -9145,7 +9145,7 @@
         <v>48</v>
       </c>
       <c r="D422" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.35">
@@ -9159,7 +9159,7 @@
         <v>48</v>
       </c>
       <c r="D423" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.35">
@@ -9173,7 +9173,7 @@
         <v>5</v>
       </c>
       <c r="D424" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.35">
@@ -9187,7 +9187,7 @@
         <v>5</v>
       </c>
       <c r="D425" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.35">
@@ -9201,7 +9201,7 @@
         <v>24</v>
       </c>
       <c r="D426" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.35">
@@ -9215,7 +9215,7 @@
         <v>5</v>
       </c>
       <c r="D427" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.35">
@@ -9229,7 +9229,7 @@
         <v>5</v>
       </c>
       <c r="D428" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.35">
@@ -9243,7 +9243,7 @@
         <v>9</v>
       </c>
       <c r="D429" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.35">
@@ -9257,7 +9257,7 @@
         <v>48</v>
       </c>
       <c r="D430" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.35">
@@ -9271,7 +9271,7 @@
         <v>24</v>
       </c>
       <c r="D431" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.35">
@@ -9285,7 +9285,7 @@
         <v>5</v>
       </c>
       <c r="D432" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.35">
@@ -9299,7 +9299,7 @@
         <v>4</v>
       </c>
       <c r="D433" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.35">
@@ -9313,7 +9313,7 @@
         <v>24</v>
       </c>
       <c r="D434" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.35">
@@ -9327,7 +9327,7 @@
         <v>5</v>
       </c>
       <c r="D435" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.35">
@@ -9341,7 +9341,7 @@
         <v>5</v>
       </c>
       <c r="D436" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.35">
@@ -9355,7 +9355,7 @@
         <v>4</v>
       </c>
       <c r="D437" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.35">
@@ -9369,7 +9369,7 @@
         <v>5</v>
       </c>
       <c r="D438" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.35">
@@ -9383,7 +9383,7 @@
         <v>5</v>
       </c>
       <c r="D439" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.35">
@@ -9397,7 +9397,7 @@
         <v>5</v>
       </c>
       <c r="D440" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.35">
@@ -9411,7 +9411,7 @@
         <v>9</v>
       </c>
       <c r="D441" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.35">
@@ -9425,7 +9425,7 @@
         <v>24</v>
       </c>
       <c r="D442" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.35">
@@ -9439,7 +9439,7 @@
         <v>5</v>
       </c>
       <c r="D443" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.35">
@@ -9453,7 +9453,7 @@
         <v>5</v>
       </c>
       <c r="D444" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.35">
@@ -9467,7 +9467,7 @@
         <v>5</v>
       </c>
       <c r="D445" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.35">
@@ -9481,7 +9481,7 @@
         <v>5</v>
       </c>
       <c r="D446" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.35">
@@ -9495,7 +9495,7 @@
         <v>24</v>
       </c>
       <c r="D447" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="448" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
@@ -9509,7 +9509,7 @@
         <v>48</v>
       </c>
       <c r="D448" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.35">
@@ -9523,7 +9523,7 @@
         <v>48</v>
       </c>
       <c r="D449" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.35">
@@ -9537,7 +9537,7 @@
         <v>48</v>
       </c>
       <c r="D450" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.35">
@@ -9551,7 +9551,7 @@
         <v>48</v>
       </c>
       <c r="D451" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.35">
@@ -9565,7 +9565,7 @@
         <v>48</v>
       </c>
       <c r="D452" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.35">
@@ -9579,7 +9579,7 @@
         <v>24</v>
       </c>
       <c r="D453" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.35">
@@ -9593,7 +9593,7 @@
         <v>4</v>
       </c>
       <c r="D454" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.35">
@@ -9607,7 +9607,7 @@
         <v>5</v>
       </c>
       <c r="D455" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.35">
@@ -9621,7 +9621,7 @@
         <v>9</v>
       </c>
       <c r="D456" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.35">
@@ -9635,7 +9635,7 @@
         <v>5</v>
       </c>
       <c r="D457" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.35">
@@ -9649,7 +9649,7 @@
         <v>5</v>
       </c>
       <c r="D458" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.35">
@@ -9663,7 +9663,7 @@
         <v>5</v>
       </c>
       <c r="D459" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.35">
@@ -9677,7 +9677,7 @@
         <v>24</v>
       </c>
       <c r="D460" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.35">
@@ -9685,13 +9685,13 @@
         <v>897</v>
       </c>
       <c r="B461" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C461" t="s">
         <v>5</v>
       </c>
       <c r="D461" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.35">
@@ -9705,7 +9705,7 @@
         <v>5</v>
       </c>
       <c r="D462" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.35">
@@ -9719,7 +9719,7 @@
         <v>5</v>
       </c>
       <c r="D463" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.35">
@@ -9733,7 +9733,7 @@
         <v>5</v>
       </c>
       <c r="D464" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.35">
@@ -9747,7 +9747,7 @@
         <v>5</v>
       </c>
       <c r="D465" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.35">
@@ -9761,7 +9761,7 @@
         <v>5</v>
       </c>
       <c r="D466" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.35">
@@ -9775,7 +9775,7 @@
         <v>5</v>
       </c>
       <c r="D467" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.35">
@@ -9789,7 +9789,7 @@
         <v>5</v>
       </c>
       <c r="D468" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.35">
@@ -9803,7 +9803,7 @@
         <v>5</v>
       </c>
       <c r="D469" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.35">
@@ -9811,153 +9811,153 @@
         <v>906</v>
       </c>
       <c r="B470" t="s">
+        <v>937</v>
+      </c>
+      <c r="C470" t="s">
+        <v>5</v>
+      </c>
+      <c r="D470" t="s">
         <v>915</v>
-      </c>
-      <c r="C470" t="s">
-        <v>5</v>
-      </c>
-      <c r="D470" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B471" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C471" t="s">
         <v>5</v>
       </c>
       <c r="D471" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B472" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C472" t="s">
         <v>5</v>
       </c>
       <c r="D472" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B473" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C473" t="s">
         <v>48</v>
       </c>
       <c r="D473" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B474" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C474" t="s">
         <v>5</v>
       </c>
       <c r="D474" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B475" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C475" t="s">
         <v>5</v>
       </c>
       <c r="D475" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B476" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C476" t="s">
         <v>48</v>
       </c>
       <c r="D476" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B477" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C477" t="s">
         <v>48</v>
       </c>
       <c r="D477" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B478" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C478" t="s">
         <v>5</v>
       </c>
       <c r="D478" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B479" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C479" t="s">
         <v>5</v>
       </c>
       <c r="D479" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B480" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C480" t="s">
         <v>5</v>
       </c>
       <c r="D480" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"added voci 5 #2"
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="999" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{512FDFA5-E790-48BA-8E82-97B517344120}"/>
+  <xr:revisionPtr revIDLastSave="1059" documentId="8_{1F1B4EF9-FC35-481D-89B7-8C2BD5E3D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE9A84B6-B868-4728-9493-CD7123797C7A}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1173">
   <si>
     <t>Griechisch</t>
   </si>
@@ -3023,9 +3023,6 @@
     <t>die Weintraube</t>
   </si>
   <si>
-    <t>ττο καρπούζι</t>
-  </si>
-  <si>
     <t>die Wassermelone</t>
   </si>
   <si>
@@ -3423,6 +3420,141 @@
   </si>
   <si>
     <t>δύσκολος, -η, -ο</t>
+  </si>
+  <si>
+    <t>το τυρί</t>
+  </si>
+  <si>
+    <t>το βούτυρο</t>
+  </si>
+  <si>
+    <t>το λάδι</t>
+  </si>
+  <si>
+    <t>το ξύδι</t>
+  </si>
+  <si>
+    <t>το ελιές</t>
+  </si>
+  <si>
+    <t>τα ζυμαρικά</t>
+  </si>
+  <si>
+    <t>το ρύζι</t>
+  </si>
+  <si>
+    <t>το αλάτι</t>
+  </si>
+  <si>
+    <t>το πιπέρι</t>
+  </si>
+  <si>
+    <t>το αυγό</t>
+  </si>
+  <si>
+    <t>η τσιπούρη</t>
+  </si>
+  <si>
+    <t>η σαρδέλη</t>
+  </si>
+  <si>
+    <t>το κοτόπουλο</t>
+  </si>
+  <si>
+    <t>τα κιμά</t>
+  </si>
+  <si>
+    <t>η μπριζόλη</t>
+  </si>
+  <si>
+    <t>το ψωμί</t>
+  </si>
+  <si>
+    <t>το κουλουράκιο</t>
+  </si>
+  <si>
+    <t>το σοκολατάκιο</t>
+  </si>
+  <si>
+    <t>το γλυκά</t>
+  </si>
+  <si>
+    <t>το παγωτό</t>
+  </si>
+  <si>
+    <t>der Käse</t>
+  </si>
+  <si>
+    <t>die Butter</t>
+  </si>
+  <si>
+    <t>das ÖL</t>
+  </si>
+  <si>
+    <t>der Essig</t>
+  </si>
+  <si>
+    <t>die Oliven</t>
+  </si>
+  <si>
+    <t>die Teigwaren</t>
+  </si>
+  <si>
+    <t>der Reis</t>
+  </si>
+  <si>
+    <t>das Salz</t>
+  </si>
+  <si>
+    <t>der Pfeffer</t>
+  </si>
+  <si>
+    <t>das Ei</t>
+  </si>
+  <si>
+    <t>die Meerbrasse</t>
+  </si>
+  <si>
+    <t>die Sardine</t>
+  </si>
+  <si>
+    <t>η γαρίδh</t>
+  </si>
+  <si>
+    <t>die Garnele</t>
+  </si>
+  <si>
+    <t>das Hühnchen</t>
+  </si>
+  <si>
+    <t>das Hackfleisch</t>
+  </si>
+  <si>
+    <t>das Kotelett</t>
+  </si>
+  <si>
+    <t>το λουκάνικo</t>
+  </si>
+  <si>
+    <t>das Würstchen</t>
+  </si>
+  <si>
+    <t>das Brot</t>
+  </si>
+  <si>
+    <t>das Plätzchen</t>
+  </si>
+  <si>
+    <t>die Praline</t>
+  </si>
+  <si>
+    <t>die Süssigkeit</t>
+  </si>
+  <si>
+    <t>das Speiseeis</t>
+  </si>
+  <si>
+    <t>το καρπούζι</t>
   </si>
 </sst>
 </file>
@@ -3462,12 +3594,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3802,10 +3933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
-  <dimension ref="A1:D577"/>
+  <dimension ref="A1:D599"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A533" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B469" sqref="B469"/>
+    <sheetView tabSelected="1" topLeftCell="A494" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A510" sqref="A510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -10228,7 +10359,7 @@
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B459" t="s">
         <v>74</v>
@@ -10689,1207 +10820,1515 @@
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A492" s="2" t="s">
+      <c r="A492" t="s">
         <v>960</v>
       </c>
-      <c r="B492" s="2" t="s">
+      <c r="B492" t="s">
         <v>961</v>
       </c>
-      <c r="C492" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D492" s="2" t="s">
-        <v>1127</v>
+      <c r="C492" t="s">
+        <v>5</v>
+      </c>
+      <c r="D492" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A493" s="2" t="s">
+      <c r="A493" t="s">
         <v>962</v>
       </c>
-      <c r="B493" s="2" t="s">
+      <c r="B493" t="s">
         <v>963</v>
       </c>
-      <c r="C493" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D493" s="2" t="s">
-        <v>1127</v>
+      <c r="C493" t="s">
+        <v>5</v>
+      </c>
+      <c r="D493" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A494" s="2" t="s">
+      <c r="A494" t="s">
         <v>964</v>
       </c>
-      <c r="B494" s="2" t="s">
+      <c r="B494" t="s">
         <v>965</v>
       </c>
-      <c r="C494" s="2" t="s">
+      <c r="C494" t="s">
         <v>47</v>
       </c>
-      <c r="D494" s="2" t="s">
-        <v>1127</v>
+      <c r="D494" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A495" s="2" t="s">
+      <c r="A495" t="s">
         <v>966</v>
       </c>
-      <c r="B495" s="2" t="s">
+      <c r="B495" t="s">
         <v>967</v>
       </c>
-      <c r="C495" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D495" s="2" t="s">
-        <v>1127</v>
+      <c r="C495" t="s">
+        <v>5</v>
+      </c>
+      <c r="D495" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A496" s="2" t="s">
+      <c r="A496" t="s">
         <v>968</v>
       </c>
-      <c r="B496" s="2" t="s">
+      <c r="B496" t="s">
         <v>969</v>
       </c>
-      <c r="C496" s="2" t="s">
+      <c r="C496" t="s">
         <v>47</v>
       </c>
-      <c r="D496" s="2" t="s">
-        <v>1127</v>
+      <c r="D496" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A497" s="2" t="s">
+      <c r="A497" t="s">
         <v>970</v>
       </c>
-      <c r="B497" s="2" t="s">
+      <c r="B497" t="s">
         <v>971</v>
       </c>
-      <c r="C497" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D497" s="2" t="s">
-        <v>1127</v>
+      <c r="C497" t="s">
+        <v>5</v>
+      </c>
+      <c r="D497" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A498" s="2" t="s">
+      <c r="A498" t="s">
         <v>972</v>
       </c>
-      <c r="B498" s="2" t="s">
+      <c r="B498" t="s">
         <v>973</v>
       </c>
-      <c r="C498" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D498" s="2" t="s">
-        <v>1127</v>
+      <c r="C498" t="s">
+        <v>5</v>
+      </c>
+      <c r="D498" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A499" s="2" t="s">
+      <c r="A499" t="s">
         <v>974</v>
       </c>
-      <c r="B499" s="2" t="s">
+      <c r="B499" t="s">
         <v>975</v>
       </c>
-      <c r="C499" s="2" t="s">
+      <c r="C499" t="s">
         <v>47</v>
       </c>
-      <c r="D499" s="2" t="s">
-        <v>1127</v>
+      <c r="D499" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A500" s="2" t="s">
+      <c r="A500" t="s">
         <v>976</v>
       </c>
-      <c r="B500" s="2" t="s">
+      <c r="B500" t="s">
         <v>31</v>
       </c>
-      <c r="C500" s="2" t="s">
+      <c r="C500" t="s">
         <v>23</v>
       </c>
-      <c r="D500" s="2" t="s">
-        <v>1127</v>
+      <c r="D500" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A501" s="2" t="s">
+      <c r="A501" t="s">
         <v>977</v>
       </c>
-      <c r="B501" s="2" t="s">
+      <c r="B501" t="s">
         <v>978</v>
       </c>
-      <c r="C501" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D501" s="2" t="s">
-        <v>1127</v>
+      <c r="C501" t="s">
+        <v>5</v>
+      </c>
+      <c r="D501" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A502" s="2" t="s">
+      <c r="A502" t="s">
         <v>979</v>
       </c>
-      <c r="B502" s="2" t="s">
+      <c r="B502" t="s">
         <v>980</v>
       </c>
-      <c r="C502" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D502" s="2" t="s">
-        <v>1127</v>
+      <c r="C502" t="s">
+        <v>5</v>
+      </c>
+      <c r="D502" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A503" s="2" t="s">
+      <c r="A503" t="s">
         <v>981</v>
       </c>
-      <c r="B503" s="2" t="s">
+      <c r="B503" t="s">
         <v>982</v>
       </c>
-      <c r="C503" s="2" t="s">
+      <c r="C503" t="s">
         <v>23</v>
       </c>
-      <c r="D503" s="2" t="s">
-        <v>1127</v>
+      <c r="D503" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A504" s="2" t="s">
+      <c r="A504" t="s">
         <v>983</v>
       </c>
-      <c r="B504" s="2" t="s">
+      <c r="B504" t="s">
         <v>984</v>
       </c>
-      <c r="C504" s="2" t="s">
+      <c r="C504" t="s">
         <v>47</v>
       </c>
-      <c r="D504" s="2" t="s">
-        <v>1127</v>
+      <c r="D504" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A505" s="2" t="s">
+      <c r="A505" t="s">
         <v>985</v>
       </c>
-      <c r="B505" s="2" t="s">
+      <c r="B505" t="s">
         <v>986</v>
       </c>
-      <c r="C505" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D505" s="2" t="s">
-        <v>1127</v>
+      <c r="C505" t="s">
+        <v>5</v>
+      </c>
+      <c r="D505" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A506" s="2" t="s">
+      <c r="A506" t="s">
         <v>987</v>
       </c>
-      <c r="B506" s="2" t="s">
+      <c r="B506" t="s">
         <v>988</v>
       </c>
-      <c r="C506" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D506" s="2" t="s">
-        <v>1127</v>
+      <c r="C506" t="s">
+        <v>5</v>
+      </c>
+      <c r="D506" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A507" s="2" t="s">
+      <c r="A507" t="s">
         <v>989</v>
       </c>
-      <c r="B507" s="2" t="s">
+      <c r="B507" t="s">
         <v>990</v>
       </c>
-      <c r="C507" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D507" s="2" t="s">
-        <v>1127</v>
+      <c r="C507" t="s">
+        <v>5</v>
+      </c>
+      <c r="D507" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A508" s="2" t="s">
+      <c r="A508" t="s">
         <v>991</v>
       </c>
-      <c r="B508" s="2" t="s">
+      <c r="B508" t="s">
         <v>992</v>
       </c>
-      <c r="C508" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D508" s="2" t="s">
-        <v>1127</v>
+      <c r="C508" t="s">
+        <v>5</v>
+      </c>
+      <c r="D508" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A509" s="2" t="s">
+      <c r="A509" t="s">
         <v>993</v>
       </c>
-      <c r="B509" s="2" t="s">
+      <c r="B509" t="s">
         <v>994</v>
       </c>
-      <c r="C509" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D509" s="2" t="s">
-        <v>1127</v>
+      <c r="C509" t="s">
+        <v>5</v>
+      </c>
+      <c r="D509" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A510" s="2" t="s">
+      <c r="A510" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B510" t="s">
         <v>995</v>
       </c>
-      <c r="B510" s="2" t="s">
+      <c r="C510" t="s">
+        <v>5</v>
+      </c>
+      <c r="D510" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A511" t="s">
         <v>996</v>
       </c>
-      <c r="C510" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D510" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="511" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A511" s="2" t="s">
+      <c r="B511" t="s">
         <v>997</v>
       </c>
-      <c r="B511" s="2" t="s">
+      <c r="C511" t="s">
+        <v>5</v>
+      </c>
+      <c r="D511" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A512" t="s">
         <v>998</v>
       </c>
-      <c r="C511" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D511" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="512" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A512" s="2" t="s">
+      <c r="B512" t="s">
         <v>999</v>
       </c>
-      <c r="B512" s="2" t="s">
+      <c r="C512" t="s">
+        <v>5</v>
+      </c>
+      <c r="D512" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A513" t="s">
         <v>1000</v>
       </c>
-      <c r="C512" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D512" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="513" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A513" s="2" t="s">
+      <c r="B513" t="s">
         <v>1001</v>
       </c>
-      <c r="B513" s="2" t="s">
+      <c r="C513" t="s">
+        <v>5</v>
+      </c>
+      <c r="D513" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A514" t="s">
         <v>1002</v>
       </c>
-      <c r="C513" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D513" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="514" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A514" s="2" t="s">
+      <c r="B514" t="s">
         <v>1003</v>
       </c>
-      <c r="B514" s="2" t="s">
+      <c r="C514" t="s">
+        <v>5</v>
+      </c>
+      <c r="D514" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A515" t="s">
         <v>1004</v>
       </c>
-      <c r="C514" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D514" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="515" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A515" s="2" t="s">
+      <c r="B515" t="s">
         <v>1005</v>
       </c>
-      <c r="B515" s="2" t="s">
+      <c r="C515" t="s">
+        <v>5</v>
+      </c>
+      <c r="D515" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A516" t="s">
         <v>1006</v>
       </c>
-      <c r="C515" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D515" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="516" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A516" s="2" t="s">
+      <c r="B516" t="s">
         <v>1007</v>
       </c>
-      <c r="B516" s="2" t="s">
+      <c r="C516" t="s">
+        <v>5</v>
+      </c>
+      <c r="D516" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A517" t="s">
         <v>1008</v>
       </c>
-      <c r="C516" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D516" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="517" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A517" s="2" t="s">
+      <c r="B517" t="s">
         <v>1009</v>
       </c>
-      <c r="B517" s="2" t="s">
+      <c r="C517" t="s">
+        <v>5</v>
+      </c>
+      <c r="D517" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A518" t="s">
         <v>1010</v>
       </c>
-      <c r="C517" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D517" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="518" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A518" s="2" t="s">
+      <c r="B518" t="s">
         <v>1011</v>
       </c>
-      <c r="B518" s="2" t="s">
+      <c r="C518" t="s">
+        <v>5</v>
+      </c>
+      <c r="D518" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A519" t="s">
         <v>1012</v>
       </c>
-      <c r="C518" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D518" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="519" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A519" s="2" t="s">
+      <c r="B519" t="s">
         <v>1013</v>
       </c>
-      <c r="B519" s="2" t="s">
+      <c r="C519" t="s">
+        <v>5</v>
+      </c>
+      <c r="D519" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A520" t="s">
         <v>1014</v>
       </c>
-      <c r="C519" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D519" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="520" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A520" s="2" t="s">
+      <c r="B520" t="s">
         <v>1015</v>
       </c>
-      <c r="B520" s="2" t="s">
+      <c r="C520" t="s">
+        <v>5</v>
+      </c>
+      <c r="D520" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A521" t="s">
         <v>1016</v>
       </c>
-      <c r="C520" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D520" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="521" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A521" s="2" t="s">
+      <c r="B521" t="s">
         <v>1017</v>
       </c>
-      <c r="B521" s="2" t="s">
+      <c r="C521" t="s">
+        <v>5</v>
+      </c>
+      <c r="D521" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A522" t="s">
         <v>1018</v>
       </c>
-      <c r="C521" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D521" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="522" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A522" s="2" t="s">
+      <c r="B522" t="s">
         <v>1019</v>
       </c>
-      <c r="B522" s="2" t="s">
+      <c r="C522" t="s">
+        <v>5</v>
+      </c>
+      <c r="D522" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A523" t="s">
         <v>1020</v>
       </c>
-      <c r="C522" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D522" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="523" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A523" s="2" t="s">
+      <c r="B523" t="s">
         <v>1021</v>
       </c>
-      <c r="B523" s="2" t="s">
+      <c r="C523" t="s">
+        <v>5</v>
+      </c>
+      <c r="D523" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A524" t="s">
         <v>1022</v>
       </c>
-      <c r="C523" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D523" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="524" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A524" s="2" t="s">
+      <c r="B524" t="s">
         <v>1023</v>
       </c>
-      <c r="B524" s="2" t="s">
+      <c r="C524" t="s">
+        <v>5</v>
+      </c>
+      <c r="D524" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A525" t="s">
         <v>1024</v>
       </c>
-      <c r="C524" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D524" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="525" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A525" s="2" t="s">
+      <c r="B525" t="s">
         <v>1025</v>
       </c>
-      <c r="B525" s="2" t="s">
+      <c r="C525" t="s">
+        <v>9</v>
+      </c>
+      <c r="D525" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A526" t="s">
         <v>1026</v>
       </c>
-      <c r="C525" s="2" t="s">
+      <c r="B526" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C526" t="s">
+        <v>5</v>
+      </c>
+      <c r="D526" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A527" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B527" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C527" t="s">
+        <v>23</v>
+      </c>
+      <c r="D527" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A528" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B528" t="s">
+        <v>869</v>
+      </c>
+      <c r="C528" t="s">
+        <v>4</v>
+      </c>
+      <c r="D528" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A529" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B529" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C529" t="s">
+        <v>5</v>
+      </c>
+      <c r="D529" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A530" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C530" t="s">
+        <v>5</v>
+      </c>
+      <c r="D530" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A531" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B531" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C531" t="s">
+        <v>5</v>
+      </c>
+      <c r="D531" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A532" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C532" t="s">
         <v>9</v>
       </c>
-      <c r="D525" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="526" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A526" s="2" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B526" s="2" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C526" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D526" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="527" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A527" s="2" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B527" s="2" t="s">
-        <v>1030</v>
-      </c>
-      <c r="C527" s="2" t="s">
+      <c r="D532" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A533" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B533" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C533" t="s">
+        <v>5</v>
+      </c>
+      <c r="D533" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A534" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B534" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C534" t="s">
+        <v>4</v>
+      </c>
+      <c r="D534" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A535" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B535" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C535" t="s">
+        <v>5</v>
+      </c>
+      <c r="D535" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A536" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B536" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C536" t="s">
+        <v>5</v>
+      </c>
+      <c r="D536" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A537" t="s">
+        <v>895</v>
+      </c>
+      <c r="B537" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C537" t="s">
+        <v>5</v>
+      </c>
+      <c r="D537" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A538" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B538" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C538" t="s">
+        <v>47</v>
+      </c>
+      <c r="D538" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A539" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C539" t="s">
+        <v>5</v>
+      </c>
+      <c r="D539" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A540" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B540" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C540" t="s">
+        <v>5</v>
+      </c>
+      <c r="D540" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A541" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B541" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C541" t="s">
         <v>23</v>
       </c>
-      <c r="D527" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="528" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A528" s="2" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B528" s="2" t="s">
-        <v>869</v>
-      </c>
-      <c r="C528" s="2" t="s">
+      <c r="D541" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A542" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B542" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C542" t="s">
+        <v>23</v>
+      </c>
+      <c r="D542" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A543" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B543" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C543" t="s">
+        <v>47</v>
+      </c>
+      <c r="D543" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A544" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B544" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C544" t="s">
+        <v>47</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A545" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B545" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C545" t="s">
+        <v>5</v>
+      </c>
+      <c r="D545" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A546" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B546" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C546" t="s">
+        <v>9</v>
+      </c>
+      <c r="D546" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A547" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B547" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C547" t="s">
+        <v>5</v>
+      </c>
+      <c r="D547" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A548" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C548" t="s">
+        <v>47</v>
+      </c>
+      <c r="D548" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A549" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B549" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C549" t="s">
+        <v>47</v>
+      </c>
+      <c r="D549" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A550" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C550" t="s">
+        <v>23</v>
+      </c>
+      <c r="D550" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A551" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C551" t="s">
+        <v>5</v>
+      </c>
+      <c r="D551" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A552" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B552" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C552" t="s">
+        <v>9</v>
+      </c>
+      <c r="D552" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A553" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C553" t="s">
+        <v>9</v>
+      </c>
+      <c r="D553" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A554" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B554" t="s">
+        <v>672</v>
+      </c>
+      <c r="C554" t="s">
+        <v>47</v>
+      </c>
+      <c r="D554" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A555" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C555" t="s">
+        <v>47</v>
+      </c>
+      <c r="D555" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A556" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B556" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C556" t="s">
+        <v>23</v>
+      </c>
+      <c r="D556" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A557" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B557" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C557" t="s">
+        <v>23</v>
+      </c>
+      <c r="D557" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A558" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C558" t="s">
         <v>4</v>
       </c>
-      <c r="D528" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="529" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A529" s="2" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B529" s="2" t="s">
-        <v>1033</v>
-      </c>
-      <c r="C529" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D529" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="530" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A530" s="2" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B530" s="2" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C530" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D530" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="531" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A531" s="2" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B531" s="2" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C531" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D531" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="532" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A532" s="2" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B532" s="2" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C532" s="2" t="s">
+      <c r="D558" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A559" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B559" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C559" t="s">
         <v>9</v>
       </c>
-      <c r="D532" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="533" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A533" s="2" t="s">
-        <v>1040</v>
-      </c>
-      <c r="B533" s="2" t="s">
-        <v>1041</v>
-      </c>
-      <c r="C533" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D533" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="534" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A534" s="2" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B534" s="2" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C534" s="2" t="s">
+      <c r="D559" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A560" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B560" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C560" t="s">
         <v>4</v>
       </c>
-      <c r="D534" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="535" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A535" s="2" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B535" s="2" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C535" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D535" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="536" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A536" s="2" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B536" s="2" t="s">
-        <v>1047</v>
-      </c>
-      <c r="C536" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D536" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="537" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A537" s="2" t="s">
-        <v>895</v>
-      </c>
-      <c r="B537" s="2" t="s">
-        <v>1048</v>
-      </c>
-      <c r="C537" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D537" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="538" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A538" s="2" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B538" s="2" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C538" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D538" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="539" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A539" s="2" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B539" s="2" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C539" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D539" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="540" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A540" s="2" t="s">
-        <v>1053</v>
-      </c>
-      <c r="B540" s="2" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C540" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D540" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="541" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A541" s="2" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B541" s="2" t="s">
-        <v>1056</v>
-      </c>
-      <c r="C541" s="2" t="s">
+      <c r="D560" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A561" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B561" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C561" t="s">
+        <v>4</v>
+      </c>
+      <c r="D561" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A562" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B562" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C562" t="s">
+        <v>5</v>
+      </c>
+      <c r="D562" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A563" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B563" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C563" t="s">
+        <v>9</v>
+      </c>
+      <c r="D563" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A564" t="s">
+        <v>729</v>
+      </c>
+      <c r="B564" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C564" t="s">
+        <v>5</v>
+      </c>
+      <c r="D564" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A565" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B565" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C565" t="s">
         <v>23</v>
       </c>
-      <c r="D541" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="542" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A542" s="2" t="s">
-        <v>1057</v>
-      </c>
-      <c r="B542" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C542" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D542" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="543" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A543" s="2" t="s">
-        <v>1059</v>
-      </c>
-      <c r="B543" s="2" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C543" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D543" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="544" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A544" s="2" t="s">
-        <v>1061</v>
-      </c>
-      <c r="B544" s="2" t="s">
-        <v>1062</v>
-      </c>
-      <c r="C544" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D544" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="545" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A545" s="2" t="s">
-        <v>1063</v>
-      </c>
-      <c r="B545" s="2" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C545" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D545" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="546" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A546" s="2" t="s">
-        <v>1065</v>
-      </c>
-      <c r="B546" s="2" t="s">
-        <v>1066</v>
-      </c>
-      <c r="C546" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D546" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="547" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A547" s="2" t="s">
-        <v>1067</v>
-      </c>
-      <c r="B547" s="2" t="s">
-        <v>1068</v>
-      </c>
-      <c r="C547" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D547" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="548" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A548" s="2" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B548" s="2" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C548" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D548" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="549" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A549" s="2" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B549" s="2" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C549" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D549" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="550" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A550" s="2" t="s">
-        <v>1073</v>
-      </c>
-      <c r="B550" s="2" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C550" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D550" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="551" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A551" s="2" t="s">
-        <v>1075</v>
-      </c>
-      <c r="B551" s="2" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C551" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D551" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="552" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A552" s="2" t="s">
-        <v>1077</v>
-      </c>
-      <c r="B552" s="2" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C552" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D552" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="553" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A553" s="2" t="s">
-        <v>1079</v>
-      </c>
-      <c r="B553" s="2" t="s">
-        <v>1080</v>
-      </c>
-      <c r="C553" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D553" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="554" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A554" s="2" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B554" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="C554" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D554" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="555" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A555" s="2" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B555" s="2" t="s">
-        <v>1083</v>
-      </c>
-      <c r="C555" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D555" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="556" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A556" s="2" t="s">
-        <v>1084</v>
-      </c>
-      <c r="B556" s="2" t="s">
-        <v>1085</v>
-      </c>
-      <c r="C556" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D556" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="557" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A557" s="2" t="s">
-        <v>1086</v>
-      </c>
-      <c r="B557" s="2" t="s">
-        <v>1087</v>
-      </c>
-      <c r="C557" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D557" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="558" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A558" s="2" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B558" s="2" t="s">
-        <v>1089</v>
-      </c>
-      <c r="C558" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D558" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="559" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A559" s="2" t="s">
-        <v>1090</v>
-      </c>
-      <c r="B559" s="2" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C559" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D559" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="560" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A560" s="2" t="s">
-        <v>1092</v>
-      </c>
-      <c r="B560" s="2" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C560" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D560" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="561" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A561" s="2" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B561" s="2" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C561" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D561" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="562" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A562" s="2" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B562" s="2" t="s">
-        <v>1097</v>
-      </c>
-      <c r="C562" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D562" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="563" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A563" s="2" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B563" s="2" t="s">
-        <v>1099</v>
-      </c>
-      <c r="C563" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D563" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="564" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A564" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="B564" s="2" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C564" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D564" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="565" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A565" s="2" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B565" s="2" t="s">
+      <c r="D565" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A566" t="s">
         <v>1102</v>
       </c>
-      <c r="C565" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D565" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="566" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A566" s="2" t="s">
+      <c r="B566" t="s">
         <v>1103</v>
       </c>
-      <c r="B566" s="2" t="s">
+      <c r="C566" t="s">
+        <v>5</v>
+      </c>
+      <c r="D566" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A567" t="s">
         <v>1104</v>
       </c>
-      <c r="C566" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D566" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="567" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A567" s="2" t="s">
+      <c r="B567" t="s">
         <v>1105</v>
       </c>
-      <c r="B567" s="2" t="s">
+      <c r="C567" t="s">
+        <v>5</v>
+      </c>
+      <c r="D567" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A568" t="s">
         <v>1106</v>
       </c>
-      <c r="C567" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D567" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="568" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A568" s="2" t="s">
+      <c r="B568" t="s">
         <v>1107</v>
       </c>
-      <c r="B568" s="2" t="s">
+      <c r="C568" t="s">
+        <v>5</v>
+      </c>
+      <c r="D568" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A569" t="s">
         <v>1108</v>
       </c>
-      <c r="C568" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D568" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="569" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A569" s="2" t="s">
+      <c r="B569" t="s">
         <v>1109</v>
       </c>
-      <c r="B569" s="2" t="s">
+      <c r="C569" t="s">
+        <v>5</v>
+      </c>
+      <c r="D569" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A570" t="s">
         <v>1110</v>
       </c>
-      <c r="C569" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D569" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="570" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A570" s="2" t="s">
+      <c r="B570" t="s">
         <v>1111</v>
       </c>
-      <c r="B570" s="2" t="s">
+      <c r="C570" t="s">
+        <v>5</v>
+      </c>
+      <c r="D570" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A571" t="s">
         <v>1112</v>
       </c>
-      <c r="C570" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D570" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="571" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A571" s="2" t="s">
+      <c r="B571" t="s">
         <v>1113</v>
       </c>
-      <c r="B571" s="2" t="s">
+      <c r="C571" t="s">
+        <v>5</v>
+      </c>
+      <c r="D571" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A572" t="s">
         <v>1114</v>
       </c>
-      <c r="C571" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D571" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="572" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A572" s="2" t="s">
+      <c r="B572" t="s">
         <v>1115</v>
       </c>
-      <c r="B572" s="2" t="s">
+      <c r="C572" t="s">
+        <v>5</v>
+      </c>
+      <c r="D572" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A573" t="s">
         <v>1116</v>
       </c>
-      <c r="C572" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D572" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="573" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A573" s="2" t="s">
+      <c r="B573" t="s">
         <v>1117</v>
       </c>
-      <c r="B573" s="2" t="s">
+      <c r="C573" t="s">
+        <v>5</v>
+      </c>
+      <c r="D573" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A574" t="s">
         <v>1118</v>
       </c>
-      <c r="C573" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D573" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="574" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A574" s="2" t="s">
+      <c r="B574" t="s">
         <v>1119</v>
       </c>
-      <c r="B574" s="2" t="s">
+      <c r="C574" t="s">
+        <v>5</v>
+      </c>
+      <c r="D574" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A575" t="s">
         <v>1120</v>
       </c>
-      <c r="C574" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D574" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="575" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A575" s="2" t="s">
+      <c r="B575" t="s">
         <v>1121</v>
       </c>
-      <c r="B575" s="2" t="s">
+      <c r="C575" t="s">
+        <v>5</v>
+      </c>
+      <c r="D575" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A576" t="s">
         <v>1122</v>
       </c>
-      <c r="C575" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D575" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="576" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A576" s="2" t="s">
+      <c r="B576" t="s">
         <v>1123</v>
       </c>
-      <c r="B576" s="2" t="s">
+      <c r="C576" t="s">
+        <v>5</v>
+      </c>
+      <c r="D576" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A577" t="s">
         <v>1124</v>
       </c>
-      <c r="C576" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D576" s="2" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="577" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A577" s="2" t="s">
+      <c r="B577" t="s">
         <v>1125</v>
       </c>
-      <c r="B577" s="2" t="s">
+      <c r="C577" t="s">
+        <v>5</v>
+      </c>
+      <c r="D577" t="s">
         <v>1126</v>
       </c>
-      <c r="C577" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D577" s="2" t="s">
-        <v>1127</v>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A578" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C578" t="s">
+        <v>5</v>
+      </c>
+      <c r="D578" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A579" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B579" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C579" t="s">
+        <v>5</v>
+      </c>
+      <c r="D579" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A580" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B580" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C580" t="s">
+        <v>5</v>
+      </c>
+      <c r="D580" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A581" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C581" t="s">
+        <v>5</v>
+      </c>
+      <c r="D581" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A582" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B582" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C582" t="s">
+        <v>5</v>
+      </c>
+      <c r="D582" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A583" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C583" t="s">
+        <v>5</v>
+      </c>
+      <c r="D583" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A584" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C584" t="s">
+        <v>5</v>
+      </c>
+      <c r="D584" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A585" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B585" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C585" t="s">
+        <v>5</v>
+      </c>
+      <c r="D585" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="586" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A586" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B586" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C586" t="s">
+        <v>5</v>
+      </c>
+      <c r="D586" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A587" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B587" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C587" t="s">
+        <v>5</v>
+      </c>
+      <c r="D587" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A588" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B588" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C588" t="s">
+        <v>5</v>
+      </c>
+      <c r="D588" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A589" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B589" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C589" t="s">
+        <v>5</v>
+      </c>
+      <c r="D589" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A590" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B590" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C590" t="s">
+        <v>5</v>
+      </c>
+      <c r="D590" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A591" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B591" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C591" t="s">
+        <v>5</v>
+      </c>
+      <c r="D591" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A592" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B592" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C592" t="s">
+        <v>5</v>
+      </c>
+      <c r="D592" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A593" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B593" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C593" t="s">
+        <v>5</v>
+      </c>
+      <c r="D593" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A594" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B594" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C594" t="s">
+        <v>5</v>
+      </c>
+      <c r="D594" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A595" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B595" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C595" t="s">
+        <v>5</v>
+      </c>
+      <c r="D595" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A596" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B596" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C596" t="s">
+        <v>5</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A597" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B597" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C597" t="s">
+        <v>5</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A598" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B598" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C598" t="s">
+        <v>5</v>
+      </c>
+      <c r="D598" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A599" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B599" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C599" t="s">
+        <v>5</v>
+      </c>
+      <c r="D599" t="s">
+        <v>1126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Voci 9 #2
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5201b5f3531a334/Desktop/Python Stuff/100 Days/1_Projects/000_Fun Stuff/00_Blackjack Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="833" documentId="13_ncr:1_{AF6E7BD2-8F9F-4013-8847-328FA9F74933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F4468C2-7342-4DAE-A915-28DB7BB1341D}"/>
+  <xr:revisionPtr revIDLastSave="838" documentId="13_ncr:1_{AF6E7BD2-8F9F-4013-8847-328FA9F74933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34571529-29F1-4854-88AE-30745C31A2A0}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" xr2:uid="{CEBB0E60-07A9-4D86-839D-390E53BA813F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3940" uniqueCount="1942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3940" uniqueCount="1943">
   <si>
     <t>Griechisch</t>
   </si>
@@ -4454,9 +4454,6 @@
     <t>Lehrbuch 7b</t>
   </si>
   <si>
-    <t>Πώς σε λένε / Πώς σας λένε?</t>
-  </si>
-  <si>
     <t>wie heisst du / wie heissen Sie?</t>
   </si>
   <si>
@@ -5744,9 +5741,6 @@
     <t>guten Appetit</t>
   </si>
   <si>
-    <t>στην υγειά σου / σας</t>
-  </si>
-  <si>
     <t>auf dein / euer Wohl!</t>
   </si>
   <si>
@@ -5865,6 +5859,15 @@
   </si>
   <si>
     <t>κυνηγάω &gt; κυνήγησα</t>
+  </si>
+  <si>
+    <t>die Sportarten</t>
+  </si>
+  <si>
+    <t>Πώς σε λένε | Πώς σας λένε?</t>
+  </si>
+  <si>
+    <t>στην υγειά σου | σας</t>
   </si>
 </sst>
 </file>
@@ -6245,8 +6248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5DAEB-82D7-45ED-9D33-FA4F48BC35C0}">
   <dimension ref="A1:D993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A965" zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A959" zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A959" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.69140625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -6266,7 +6269,7 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -7237,10 +7240,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B71" t="s">
         <v>1471</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1472</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -7335,7 +7338,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -7349,7 +7352,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B79" t="s">
         <v>11</v>
@@ -7363,7 +7366,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B80" t="s">
         <v>14</v>
@@ -7377,7 +7380,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
@@ -7391,7 +7394,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B82" t="s">
         <v>24</v>
@@ -7405,7 +7408,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B83" t="s">
         <v>28</v>
@@ -7419,7 +7422,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B84" t="s">
         <v>29</v>
@@ -7433,7 +7436,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B85" t="s">
         <v>33</v>
@@ -7447,7 +7450,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B86" t="s">
         <v>35</v>
@@ -7461,7 +7464,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B87" t="s">
         <v>37</v>
@@ -7475,7 +7478,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B88" t="s">
         <v>39</v>
@@ -7489,7 +7492,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B89" t="s">
         <v>41</v>
@@ -7503,7 +7506,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B90" t="s">
         <v>47</v>
@@ -7517,7 +7520,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B91" t="s">
         <v>51</v>
@@ -7531,7 +7534,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B92" t="s">
         <v>59</v>
@@ -7545,7 +7548,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B93" t="s">
         <v>61</v>
@@ -7559,7 +7562,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="B94" t="s">
         <v>64</v>
@@ -7573,7 +7576,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="B95" t="s">
         <v>67</v>
@@ -7587,7 +7590,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="B96" t="s">
         <v>74</v>
@@ -9519,7 +9522,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="B234" t="s">
         <v>211</v>
@@ -9533,7 +9536,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B235" t="s">
         <v>216</v>
@@ -9547,7 +9550,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="B236" t="s">
         <v>219</v>
@@ -9561,7 +9564,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="B237" t="s">
         <v>229</v>
@@ -9575,7 +9578,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="B238" t="s">
         <v>241</v>
@@ -9589,7 +9592,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="B239" t="s">
         <v>244</v>
@@ -9617,7 +9620,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B241" t="s">
         <v>252</v>
@@ -9631,7 +9634,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="B242" t="s">
         <v>269</v>
@@ -9645,7 +9648,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="B243" t="s">
         <v>276</v>
@@ -9687,7 +9690,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="B246" t="s">
         <v>293</v>
@@ -9701,7 +9704,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="B247" t="s">
         <v>302</v>
@@ -9715,7 +9718,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="B248" t="s">
         <v>305</v>
@@ -9729,7 +9732,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="B249" t="s">
         <v>310</v>
@@ -9743,7 +9746,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="B250" t="s">
         <v>313</v>
@@ -9757,7 +9760,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="B251" t="s">
         <v>335</v>
@@ -9771,7 +9774,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="B252" t="s">
         <v>338</v>
@@ -9785,7 +9788,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="B253" t="s">
         <v>359</v>
@@ -9799,7 +9802,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="B254" t="s">
         <v>362</v>
@@ -10009,7 +10012,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B269" t="s">
         <v>530</v>
@@ -10429,7 +10432,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="B299" t="s">
         <v>562</v>
@@ -10849,7 +10852,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="B329" t="s">
         <v>621</v>
@@ -10863,7 +10866,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="B330" t="s">
         <v>622</v>
@@ -10947,7 +10950,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="B336" t="s">
         <v>628</v>
@@ -11129,7 +11132,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="B349" t="s">
         <v>640</v>
@@ -11143,7 +11146,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="B350" t="s">
         <v>641</v>
@@ -12417,7 +12420,7 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="B441" t="s">
         <v>808</v>
@@ -12473,7 +12476,7 @@
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="B445" t="s">
         <v>812</v>
@@ -12725,7 +12728,7 @@
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="B463" t="s">
         <v>828</v>
@@ -13607,7 +13610,7 @@
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="B526" t="s">
         <v>812</v>
@@ -13691,7 +13694,7 @@
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B532" t="s">
         <v>982</v>
@@ -14027,7 +14030,7 @@
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B556" t="s">
         <v>1027</v>
@@ -14055,7 +14058,7 @@
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B558" t="s">
         <v>1030</v>
@@ -14069,7 +14072,7 @@
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B559" t="s">
         <v>1031</v>
@@ -14783,7 +14786,7 @@
     </row>
     <row r="610" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B610" t="s">
         <v>1132</v>
@@ -14825,7 +14828,7 @@
     </row>
     <row r="613" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B613" t="s">
         <v>1137</v>
@@ -14951,7 +14954,7 @@
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B622" t="s">
         <v>1153</v>
@@ -14993,7 +14996,7 @@
     </row>
     <row r="625" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B625" t="s">
         <v>1157</v>
@@ -15021,7 +15024,7 @@
     </row>
     <row r="627" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B627" t="s">
         <v>1160</v>
@@ -15035,7 +15038,7 @@
     </row>
     <row r="628" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B628" t="s">
         <v>1161</v>
@@ -15091,7 +15094,7 @@
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B632" t="s">
         <v>1168</v>
@@ -15217,7 +15220,7 @@
     </row>
     <row r="641" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B641" t="s">
         <v>1184</v>
@@ -15231,7 +15234,7 @@
     </row>
     <row r="642" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B642" t="s">
         <v>1185</v>
@@ -15399,7 +15402,7 @@
     </row>
     <row r="654" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B654" t="s">
         <v>1208</v>
@@ -15413,7 +15416,7 @@
     </row>
     <row r="655" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B655" t="s">
         <v>1209</v>
@@ -15511,7 +15514,7 @@
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B662" t="s">
         <v>1218</v>
@@ -15553,7 +15556,7 @@
     </row>
     <row r="665" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A665" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B665" t="s">
         <v>1222</v>
@@ -15959,7 +15962,7 @@
     </row>
     <row r="694" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B694" t="s">
         <v>1447</v>
@@ -16001,7 +16004,7 @@
     </row>
     <row r="697" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="B697" t="s">
         <v>1443</v>
@@ -16141,7 +16144,7 @@
     </row>
     <row r="707" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B707" t="s">
         <v>1424</v>
@@ -16183,7 +16186,7 @@
     </row>
     <row r="710" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B710" t="s">
         <v>1419</v>
@@ -16337,7 +16340,7 @@
     </row>
     <row r="721" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B721" t="s">
         <v>1399</v>
@@ -16379,7 +16382,7 @@
     </row>
     <row r="724" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B724" t="s">
         <v>1394</v>
@@ -16463,7 +16466,7 @@
     </row>
     <row r="730" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A730" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B730" t="s">
         <v>1385</v>
@@ -16547,7 +16550,7 @@
     </row>
     <row r="736" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A736" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B736" t="s">
         <v>1374</v>
@@ -16603,7 +16606,7 @@
     </row>
     <row r="740" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A740" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B740" t="s">
         <v>1367</v>
@@ -16729,7 +16732,7 @@
     </row>
     <row r="749" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A749" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B749" t="s">
         <v>1351</v>
@@ -16827,7 +16830,7 @@
     </row>
     <row r="756" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A756" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="B756" t="s">
         <v>1338</v>
@@ -16841,7 +16844,7 @@
     </row>
     <row r="757" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A757" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B757" t="s">
         <v>1337</v>
@@ -16855,7 +16858,7 @@
     </row>
     <row r="758" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A758" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="B758" t="s">
         <v>1336</v>
@@ -17345,413 +17348,413 @@
     </row>
     <row r="793" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B793" t="s">
         <v>1474</v>
-      </c>
-      <c r="B793" t="s">
-        <v>1475</v>
       </c>
       <c r="C793" t="s">
         <v>22</v>
       </c>
       <c r="D793" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="794" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="B794" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C794" t="s">
         <v>4</v>
       </c>
       <c r="D794" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="795" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B795" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="C795" t="s">
         <v>4</v>
       </c>
       <c r="D795" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="796" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A796" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B796" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="C796" t="s">
         <v>4</v>
       </c>
       <c r="D796" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="797" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A797" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B797" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="C797" t="s">
         <v>3</v>
       </c>
       <c r="D797" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="798" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A798" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B798" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="C798" t="s">
         <v>4</v>
       </c>
       <c r="D798" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="799" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A799" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B799" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="C799" t="s">
         <v>45</v>
       </c>
       <c r="D799" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="800" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A800" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B800" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="C800" t="s">
         <v>4</v>
       </c>
       <c r="D800" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="801" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A801" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B801" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="C801" t="s">
         <v>4</v>
       </c>
       <c r="D801" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="802" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A802" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B802" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="C802" t="s">
         <v>3</v>
       </c>
       <c r="D802" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="803" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A803" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B803" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C803" t="s">
         <v>22</v>
       </c>
       <c r="D803" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="804" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="B804" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C804" t="s">
         <v>3</v>
       </c>
       <c r="D804" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="805" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="B805" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C805" t="s">
         <v>3</v>
       </c>
       <c r="D805" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="806" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="B806" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C806" t="s">
         <v>3</v>
       </c>
       <c r="D806" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="807" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B807" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C807" t="s">
         <v>4</v>
       </c>
       <c r="D807" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="808" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="B808" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C808" t="s">
         <v>4</v>
       </c>
       <c r="D808" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="809" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="B809" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C809" t="s">
         <v>4</v>
       </c>
       <c r="D809" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="810" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="B810" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C810" t="s">
         <v>3</v>
       </c>
       <c r="D810" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="811" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B811" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C811" t="s">
         <v>4</v>
       </c>
       <c r="D811" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="812" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B812" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C812" t="s">
         <v>4</v>
       </c>
       <c r="D812" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="813" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="B813" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C813" t="s">
         <v>4</v>
       </c>
       <c r="D813" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="814" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B814" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C814" t="s">
         <v>3</v>
       </c>
       <c r="D814" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="815" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="B815" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C815" t="s">
         <v>4</v>
       </c>
       <c r="D815" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="816" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="B816" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C816" t="s">
         <v>4</v>
       </c>
       <c r="D816" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="817" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A817" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B817" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C817" t="s">
         <v>4</v>
       </c>
       <c r="D817" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="818" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A818" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B818" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C818" t="s">
         <v>4</v>
       </c>
       <c r="D818" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="819" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A819" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="B819" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C819" t="s">
         <v>22</v>
       </c>
       <c r="D819" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="820" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="B820" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C820" t="s">
         <v>3</v>
       </c>
       <c r="D820" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="821" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A821" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="B821" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C821" t="s">
         <v>3</v>
       </c>
       <c r="D821" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="822" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A822" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="B822" t="s">
         <v>621</v>
@@ -17760,348 +17763,348 @@
         <v>3</v>
       </c>
       <c r="D822" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="823" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A823" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B823" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C823" t="s">
         <v>4</v>
       </c>
       <c r="D823" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="824" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A824" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B824" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C824" t="s">
         <v>4</v>
       </c>
       <c r="D824" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="825" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A825" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B825" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C825" t="s">
         <v>8</v>
       </c>
       <c r="D825" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="826" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A826" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="B826" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C826" t="s">
         <v>4</v>
       </c>
       <c r="D826" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="827" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A827" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="B827" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C827" t="s">
         <v>3</v>
       </c>
       <c r="D827" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="828" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A828" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B828" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C828" t="s">
         <v>4</v>
       </c>
       <c r="D828" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A829" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="B829" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C829" t="s">
         <v>3</v>
       </c>
       <c r="D829" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="830" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A830" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B830" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C830" t="s">
         <v>45</v>
       </c>
       <c r="D830" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A831" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B831" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C831" t="s">
         <v>4</v>
       </c>
       <c r="D831" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="832" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A832" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B832" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C832" t="s">
         <v>4</v>
       </c>
       <c r="D832" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A833" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B833" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C833" t="s">
         <v>4</v>
       </c>
       <c r="D833" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A834" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B834" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C834" t="s">
         <v>3</v>
       </c>
       <c r="D834" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="835" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A835" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B835" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C835" t="s">
         <v>45</v>
       </c>
       <c r="D835" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="836" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A836" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B836" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C836" t="s">
         <v>4</v>
       </c>
       <c r="D836" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="837" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A837" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="B837" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="C837" t="s">
         <v>3</v>
       </c>
       <c r="D837" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A838" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B838" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C838" t="s">
         <v>3</v>
       </c>
       <c r="D838" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A839" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B839" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="C839" t="s">
         <v>45</v>
       </c>
       <c r="D839" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A840" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B840" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C840" t="s">
         <v>658</v>
       </c>
       <c r="D840" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A841" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B841" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="C841" t="s">
         <v>45</v>
       </c>
       <c r="D841" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A842" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B842" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="C842" t="s">
         <v>22</v>
       </c>
       <c r="D842" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="843" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A843" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B843" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="C843" t="s">
         <v>3</v>
       </c>
       <c r="D843" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="844" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A844" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="B844" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="C844" t="s">
         <v>3</v>
       </c>
       <c r="D844" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="845" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A845" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B845" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="C845" t="s">
         <v>45</v>
       </c>
       <c r="D845" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="846" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A846" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B846" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C846" t="s">
         <v>22</v>
       </c>
       <c r="D846" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A847" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="B847" t="s">
         <v>778</v>
@@ -18110,147 +18113,147 @@
         <v>4</v>
       </c>
       <c r="D847" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="848" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A848" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="B848" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C848" t="s">
         <v>3</v>
       </c>
       <c r="D848" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="849" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A849" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="B849" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="C849" t="s">
         <v>45</v>
       </c>
       <c r="D849" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="850" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A850" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B850" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="C850" t="s">
         <v>4</v>
       </c>
       <c r="D850" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="851" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A851" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B851" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C851" t="s">
         <v>4</v>
       </c>
       <c r="D851" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="852" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A852" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B852" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="C852" t="s">
         <v>22</v>
       </c>
       <c r="D852" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A853" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="B853" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="C853" t="s">
         <v>4</v>
       </c>
       <c r="D853" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="854" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A854" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="B854" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C854" t="s">
         <v>4</v>
       </c>
       <c r="D854" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="855" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A855" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B855" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="C855" t="s">
         <v>3</v>
       </c>
       <c r="D855" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="856" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A856" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="B856" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="C856" t="s">
         <v>3</v>
       </c>
       <c r="D856" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="857" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B857" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="C857" t="s">
         <v>22</v>
       </c>
       <c r="D857" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="858" spans="1:4" x14ac:dyDescent="0.3">
@@ -18258,116 +18261,116 @@
         <v>667</v>
       </c>
       <c r="B858" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="C858" t="s">
         <v>4</v>
       </c>
       <c r="D858" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="859" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B859" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="C859" t="s">
         <v>22</v>
       </c>
       <c r="D859" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="860" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A860" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B860" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C860" t="s">
         <v>45</v>
       </c>
       <c r="D860" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="861" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A861" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B861" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C861" t="s">
         <v>4</v>
       </c>
       <c r="D861" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="862" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A862" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B862" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C862" t="s">
         <v>4</v>
       </c>
       <c r="D862" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="863" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A863" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B863" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C863" t="s">
         <v>4</v>
       </c>
       <c r="D863" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="864" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A864" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B864" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C864" t="s">
         <v>4</v>
       </c>
       <c r="D864" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="865" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A865" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="B865" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C865" t="s">
         <v>3</v>
       </c>
       <c r="D865" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="866" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A866" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B866" t="s">
         <v>63</v>
@@ -18376,12 +18379,12 @@
         <v>22</v>
       </c>
       <c r="D866" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="867" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A867" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B867" t="s">
         <v>40</v>
@@ -18390,1202 +18393,1202 @@
         <v>45</v>
       </c>
       <c r="D867" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="868" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A868" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B868" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C868" t="s">
         <v>4</v>
       </c>
       <c r="D868" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="869" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A869" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B869" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C869" t="s">
         <v>3</v>
       </c>
       <c r="D869" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="870" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A870" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="B870" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C870" t="s">
         <v>22</v>
       </c>
       <c r="D870" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="871" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="B871" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C871" t="s">
         <v>3</v>
       </c>
       <c r="D871" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="872" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="B872" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C872" t="s">
         <v>4</v>
       </c>
       <c r="D872" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="873" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="B873" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C873" t="s">
         <v>4</v>
       </c>
       <c r="D873" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="874" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="B874" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C874" t="s">
         <v>4</v>
       </c>
       <c r="D874" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="875" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B875" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C875" t="s">
         <v>4</v>
       </c>
       <c r="D875" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="876" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B876" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C876" t="s">
         <v>4</v>
       </c>
       <c r="D876" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="877" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B877" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C877" t="s">
         <v>4</v>
       </c>
       <c r="D877" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="878" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B878" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C878" t="s">
         <v>4</v>
       </c>
       <c r="D878" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="879" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B879" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="C879" t="s">
         <v>4</v>
       </c>
       <c r="D879" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="880" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A880" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B880" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C880" t="s">
         <v>4</v>
       </c>
       <c r="D880" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="881" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A881" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B881" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C881" t="s">
         <v>3</v>
       </c>
       <c r="D881" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="882" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="B882" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C882" t="s">
         <v>658</v>
       </c>
       <c r="D882" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="883" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A883" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="B883" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C883" t="s">
         <v>658</v>
       </c>
       <c r="D883" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="884" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A884" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B884" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="C884" t="s">
         <v>658</v>
       </c>
       <c r="D884" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="885" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A885" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="B885" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="C885" t="s">
         <v>658</v>
       </c>
       <c r="D885" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="886" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A886" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="B886" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="C886" t="s">
         <v>658</v>
       </c>
       <c r="D886" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="887" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A887" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="B887" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="C887" t="s">
         <v>658</v>
       </c>
       <c r="D887" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="888" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A888" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="B888" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C888" t="s">
         <v>658</v>
       </c>
       <c r="D888" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="889" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A889" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="B889" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C889" t="s">
         <v>658</v>
       </c>
       <c r="D889" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="890" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A890" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B890" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C890" t="s">
         <v>658</v>
       </c>
       <c r="D890" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="891" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A891" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="B891" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C891" t="s">
         <v>658</v>
       </c>
       <c r="D891" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="892" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A892" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="B892" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="C892" t="s">
         <v>658</v>
       </c>
       <c r="D892" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="893" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A893" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B893" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="C893" t="s">
         <v>658</v>
       </c>
       <c r="D893" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="894" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A894" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B894" t="s">
         <v>1743</v>
-      </c>
-      <c r="B894" t="s">
-        <v>1744</v>
       </c>
       <c r="C894" t="s">
         <v>22</v>
       </c>
       <c r="D894" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="895" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A895" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B895" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="C895" t="s">
         <v>4</v>
       </c>
       <c r="D895" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="896" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B896" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="C896" t="s">
         <v>4</v>
       </c>
       <c r="D896" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="897" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A897" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="B897" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="C897" t="s">
         <v>4</v>
       </c>
       <c r="D897" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="898" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A898" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="B898" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="C898" t="s">
         <v>4</v>
       </c>
       <c r="D898" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="899" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A899" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B899" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="C899" t="s">
         <v>4</v>
       </c>
       <c r="D899" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="900" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A900" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B900" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="C900" t="s">
         <v>4</v>
       </c>
       <c r="D900" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="901" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A901" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="B901" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="C901" t="s">
         <v>4</v>
       </c>
       <c r="D901" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="902" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A902" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="B902" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C902" t="s">
         <v>4</v>
       </c>
       <c r="D902" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="903" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A903" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B903" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="C903" t="s">
         <v>4</v>
       </c>
       <c r="D903" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="904" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="B904" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C904" t="s">
         <v>3</v>
       </c>
       <c r="D904" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="905" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A905" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B905" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="C905" t="s">
         <v>4</v>
       </c>
       <c r="D905" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="906" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A906" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="B906" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="C906" t="s">
         <v>45</v>
       </c>
       <c r="D906" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="907" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A907" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="B907" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="C907" t="s">
         <v>3</v>
       </c>
       <c r="D907" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="908" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A908" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B908" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="C908" t="s">
         <v>4</v>
       </c>
       <c r="D908" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="909" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A909" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B909" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="C909" t="s">
         <v>45</v>
       </c>
       <c r="D909" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="910" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A910" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B910" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="C910" t="s">
         <v>4</v>
       </c>
       <c r="D910" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="911" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A911" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="B911" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="C911" t="s">
         <v>45</v>
       </c>
       <c r="D911" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="912" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A912" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="B912" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="C912" t="s">
         <v>4</v>
       </c>
       <c r="D912" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="913" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A913" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B913" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="C913" t="s">
         <v>4</v>
       </c>
       <c r="D913" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="914" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A914" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B914" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="C914" t="s">
         <v>4</v>
       </c>
       <c r="D914" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="915" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A915" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B915" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="C915" t="s">
         <v>4</v>
       </c>
       <c r="D915" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="916" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A916" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="B916" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="C916" t="s">
         <v>45</v>
       </c>
       <c r="D916" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="917" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A917" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="B917" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="C917" t="s">
         <v>4</v>
       </c>
       <c r="D917" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="918" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A918" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="B918" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="C918" t="s">
         <v>22</v>
       </c>
       <c r="D918" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="919" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A919" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="B919" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="C919" t="s">
         <v>4</v>
       </c>
       <c r="D919" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="920" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B920" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="C920" t="s">
         <v>4</v>
       </c>
       <c r="D920" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="921" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A921" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="B921" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="C921" t="s">
         <v>45</v>
       </c>
       <c r="D921" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="922" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A922" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="B922" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C922" t="s">
         <v>4</v>
       </c>
       <c r="D922" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="923" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A923" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B923" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="C923" t="s">
         <v>4</v>
       </c>
       <c r="D923" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="924" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A924" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="B924" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="C924" t="s">
         <v>4</v>
       </c>
       <c r="D924" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="925" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="B925" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="C925" t="s">
         <v>3</v>
       </c>
       <c r="D925" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="926" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A926" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="B926" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="C926" t="s">
         <v>4</v>
       </c>
       <c r="D926" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="927" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A927" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B927" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="C927" t="s">
         <v>4</v>
       </c>
       <c r="D927" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="928" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A928" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B928" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="C928" t="s">
         <v>45</v>
       </c>
       <c r="D928" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="929" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A929" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B929" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="C929" t="s">
         <v>4</v>
       </c>
       <c r="D929" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="930" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A930" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="B930" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="C930" t="s">
         <v>3</v>
       </c>
       <c r="D930" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="931" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A931" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B931" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="C931" t="s">
         <v>4</v>
       </c>
       <c r="D931" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="932" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A932" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="B932" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="C932" t="s">
         <v>3</v>
       </c>
       <c r="D932" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="933" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A933" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="B933" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="C933" t="s">
         <v>45</v>
       </c>
       <c r="D933" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="934" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A934" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B934" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="C934" t="s">
         <v>8</v>
       </c>
       <c r="D934" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="935" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A935" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B935" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="C935" t="s">
         <v>4</v>
       </c>
       <c r="D935" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="936" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A936" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B936" t="s">
         <v>1862</v>
       </c>
-      <c r="B936" t="s">
-        <v>1863</v>
-      </c>
       <c r="C936" t="s">
         <v>4</v>
       </c>
       <c r="D936" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="937" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A937" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B937" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="C937" t="s">
         <v>658</v>
       </c>
       <c r="D937" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="938" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A938" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B938" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="C938" t="s">
         <v>4</v>
       </c>
       <c r="D938" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="939" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A939" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B939" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="C939" t="s">
         <v>8</v>
       </c>
       <c r="D939" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="940" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A940" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
       <c r="B940" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="C940" t="s">
         <v>3</v>
       </c>
       <c r="D940" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="941" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A941" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B941" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="C941" t="s">
         <v>4</v>
       </c>
       <c r="D941" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="942" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="B942" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="C942" t="s">
         <v>4</v>
       </c>
       <c r="D942" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="943" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A943" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B943" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="C943" t="s">
         <v>22</v>
       </c>
       <c r="D943" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="944" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A944" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B944" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="C944" t="s">
         <v>4</v>
       </c>
       <c r="D944" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="945" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A945" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B945" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="C945" t="s">
         <v>4</v>
       </c>
       <c r="D945" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="946" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A946" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B946" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="C946" t="s">
         <v>4</v>
       </c>
       <c r="D946" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="947" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A947" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="B947" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="C947" t="s">
         <v>4</v>
       </c>
       <c r="D947" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="948" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A948" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="B948" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="C948" t="s">
         <v>4</v>
       </c>
       <c r="D948" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="949" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A949" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="B949" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="C949" t="s">
         <v>3</v>
       </c>
       <c r="D949" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="950" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A950" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="B950" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="C950" t="s">
         <v>4</v>
       </c>
       <c r="D950" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="951" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A951" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B951" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="C951" t="s">
         <v>4</v>
       </c>
       <c r="D951" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="952" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A952" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B952" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="C952" t="s">
         <v>4</v>
       </c>
       <c r="D952" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="953" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A953" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B953" t="s">
         <v>1101</v>
@@ -19594,567 +19597,567 @@
         <v>4</v>
       </c>
       <c r="D953" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="954" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A954" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B954" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="C954" t="s">
         <v>4</v>
       </c>
       <c r="D954" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="955" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A955" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B955" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="C955" t="s">
         <v>4</v>
       </c>
       <c r="D955" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="956" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A956" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="B956" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="C956" t="s">
         <v>3</v>
       </c>
       <c r="D956" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="957" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A957" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B957" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="C957" t="s">
         <v>22</v>
       </c>
       <c r="D957" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="958" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A958" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="B958" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="C958" t="s">
         <v>45</v>
       </c>
       <c r="D958" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="959" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A959" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B959" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="C959" t="s">
         <v>4</v>
       </c>
       <c r="D959" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="960" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A960" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="B960" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="C960" t="s">
         <v>45</v>
       </c>
       <c r="D960" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="961" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A961" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="B961" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="C961" t="s">
         <v>3</v>
       </c>
       <c r="D961" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="962" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A962" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B962" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="C962" t="s">
         <v>4</v>
       </c>
       <c r="D962" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="963" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A963" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B963" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="C963" t="s">
         <v>658</v>
       </c>
       <c r="D963" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="964" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A964" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="B964" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="C964" t="s">
         <v>3</v>
       </c>
       <c r="D964" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="965" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A965" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B965" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="C965" t="s">
         <v>4</v>
       </c>
       <c r="D965" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="966" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A966" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B966" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="C966" t="s">
         <v>4</v>
       </c>
       <c r="D966" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="967" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A967" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B967" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="C967" t="s">
         <v>4</v>
       </c>
       <c r="D967" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="968" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A968" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B968" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="C968" t="s">
         <v>4</v>
       </c>
       <c r="D968" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="969" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A969" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B969" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="C969" t="s">
         <v>4</v>
       </c>
       <c r="D969" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="970" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A970" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B970" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="C970" t="s">
         <v>4</v>
       </c>
       <c r="D970" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="971" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A971" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B971" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="C971" t="s">
         <v>4</v>
       </c>
       <c r="D971" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="972" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A972" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B972" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="C972" t="s">
         <v>4</v>
       </c>
       <c r="D972" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="973" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A973" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B973" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="C973" t="s">
         <v>4</v>
       </c>
       <c r="D973" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="974" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A974" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B974" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="C974" t="s">
         <v>22</v>
       </c>
       <c r="D974" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="975" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A975" t="s">
-        <v>1901</v>
+        <v>1942</v>
       </c>
       <c r="B975" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="C975" t="s">
         <v>8</v>
       </c>
       <c r="D975" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="976" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A976" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="B976" t="s">
-        <v>1875</v>
+        <v>1940</v>
       </c>
       <c r="C976" t="s">
         <v>4</v>
       </c>
       <c r="D976" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="977" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A977" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B977" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
       <c r="C977" t="s">
         <v>4</v>
       </c>
       <c r="D977" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="978" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A978" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="B978" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="C978" t="s">
         <v>3</v>
       </c>
       <c r="D978" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="979" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A979" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B979" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="C979" t="s">
         <v>4</v>
       </c>
       <c r="D979" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="980" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A980" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="B980" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="C980" t="s">
         <v>3</v>
       </c>
       <c r="D980" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="981" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A981" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="B981" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="C981" t="s">
         <v>4</v>
       </c>
       <c r="D981" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="982" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A982" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="B982" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
       <c r="C982" t="s">
         <v>3</v>
       </c>
       <c r="D982" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="983" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A983" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B983" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="C983" t="s">
         <v>4</v>
       </c>
       <c r="D983" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="984" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A984" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B984" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="C984" t="s">
         <v>4</v>
       </c>
       <c r="D984" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="985" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A985" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="B985" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="C985" t="s">
         <v>4</v>
       </c>
       <c r="D985" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="986" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A986" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="B986" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="C986" t="s">
         <v>4</v>
       </c>
       <c r="D986" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="987" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A987" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B987" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="C987" t="s">
         <v>3</v>
       </c>
       <c r="D987" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="988" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A988" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B988" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="C988" t="s">
         <v>4</v>
       </c>
       <c r="D988" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="989" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A989" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B989" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="C989" t="s">
         <v>3</v>
       </c>
       <c r="D989" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="990" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A990" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B990" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="C990" t="s">
         <v>4</v>
       </c>
       <c r="D990" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="991" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A991" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B991" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="C991" t="s">
         <v>3</v>
       </c>
       <c r="D991" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="992" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A992" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="B992" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="C992" t="s">
         <v>4</v>
       </c>
       <c r="D992" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="993" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A993" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B993" t="s">
         <v>1819</v>
-      </c>
-      <c r="B993" t="s">
-        <v>1820</v>
       </c>
       <c r="C993" t="s">
         <v>3</v>
       </c>
       <c r="D993" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>